<commit_message>
Update all documentation including Excel, diagrams, README
</commit_message>
<xml_diff>
--- a/data/methodology/data-extraction/data.xlsx
+++ b/data/methodology/data-extraction/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sousa\Dev\slr-ltlm-mr\data\methodology\data-extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0B1301-9D99-446A-A5B9-C7597EC60F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827F31F9-1895-4418-8612-42835B391C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10217,6 +10217,674 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="147">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -11022,729 +11690,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE2EFDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFE2EFDA"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -12131,6 +12076,61 @@
       </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE2EFDA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFE2EFDA"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -12182,85 +12182,85 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{56D3EF4C-CF38-43EE-92A7-7FB5EF4F04C8}" name="Table2" displayName="Table2" ref="A2:R412" tableType="queryTable" totalsRowShown="0" headerRowDxfId="146" dataDxfId="145">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{56D3EF4C-CF38-43EE-92A7-7FB5EF4F04C8}" name="Table2" displayName="Table2" ref="A2:R412" tableType="queryTable" totalsRowShown="0" headerRowDxfId="139" dataDxfId="138">
   <autoFilter ref="A2:R412" xr:uid="{56D3EF4C-CF38-43EE-92A7-7FB5EF4F04C8}"/>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{F866BBA7-4AC0-456D-8BF6-CACF37853E53}" uniqueName="1" name="title" queryTableFieldId="1" dataDxfId="144"/>
-    <tableColumn id="18" xr3:uid="{A2826505-190A-4FED-8DA4-C03F8C9FF3F3}" uniqueName="18" name="author" queryTableFieldId="18" dataDxfId="143"/>
-    <tableColumn id="2" xr3:uid="{5DCCBB1E-D51F-4A0D-88EA-708103469CAF}" uniqueName="2" name="year" queryTableFieldId="2" dataDxfId="142"/>
-    <tableColumn id="3" xr3:uid="{6DC2321A-EBF3-4A2F-88E3-4B73262A82B8}" uniqueName="3" name="doi" queryTableFieldId="3" dataDxfId="141"/>
-    <tableColumn id="4" xr3:uid="{E980E7C7-406F-4054-87FB-C887DB4B2053}" uniqueName="4" name="url" queryTableFieldId="4" dataDxfId="140"/>
-    <tableColumn id="5" xr3:uid="{34B81B81-EF76-4B54-9237-7AE334AE5578}" uniqueName="5" name="QE parsifal" queryTableFieldId="5" dataDxfId="139"/>
-    <tableColumn id="6" xr3:uid="{594389FB-04A3-4161-B257-EB1DCD730101}" uniqueName="6" name="QE1: related" queryTableFieldId="6" dataDxfId="138"/>
-    <tableColumn id="7" xr3:uid="{0BA238F0-F4F9-4FFE-86B0-8A756146C8D8}" uniqueName="7" name="QE2: method" queryTableFieldId="7" dataDxfId="137"/>
-    <tableColumn id="8" xr3:uid="{C0EB6FEC-D203-4F01-B584-34FE796F2635}" uniqueName="8" name="QE3: l+m" queryTableFieldId="8" dataDxfId="136"/>
-    <tableColumn id="9" xr3:uid="{02418B78-D38A-4642-9393-8AE6F8A5608E}" uniqueName="9" name="QE4: hw+sw" queryTableFieldId="9" dataDxfId="135"/>
-    <tableColumn id="10" xr3:uid="{936B3ED9-F496-4CA5-B86E-E7BA2F308011}" uniqueName="10" name="QE5: long" queryTableFieldId="10" dataDxfId="134"/>
-    <tableColumn id="11" xr3:uid="{76A8C7B4-55B1-4FEB-86A4-19383EA76E7C}" uniqueName="11" name="QE6: others" queryTableFieldId="11" dataDxfId="133"/>
-    <tableColumn id="12" xr3:uid="{1C2CDAEC-857E-46D9-9B69-F4223179257E}" uniqueName="12" name="QE7: public" queryTableFieldId="12" dataDxfId="132"/>
-    <tableColumn id="13" xr3:uid="{4F68A5A7-4AA7-4BBE-93D6-B0B04FD21540}" uniqueName="13" name="QE8: results" queryTableFieldId="13" dataDxfId="131"/>
-    <tableColumn id="14" xr3:uid="{53191D3F-4AC6-4545-B9D6-5191F2222E34}" uniqueName="14" name="QE score" queryTableFieldId="14" dataDxfId="130"/>
-    <tableColumn id="15" xr3:uid="{B1CE6676-AE3F-4BB8-8DC2-32E78F35A19D}" uniqueName="15" name="QE R1:_x000a_QE2/3/5/8" queryTableFieldId="15" dataDxfId="129"/>
-    <tableColumn id="16" xr3:uid="{6AEE4540-681E-42C3-8C64-F84A057E3B2D}" uniqueName="16" name="QE R2:_x000a_cut-off" queryTableFieldId="16" dataDxfId="128"/>
-    <tableColumn id="17" xr3:uid="{8F38DD26-0C87-4DBC-83F8-E3801205D195}" uniqueName="17" name="include?" queryTableFieldId="17" dataDxfId="127"/>
+    <tableColumn id="1" xr3:uid="{F866BBA7-4AC0-456D-8BF6-CACF37853E53}" uniqueName="1" name="title" queryTableFieldId="1" dataDxfId="137"/>
+    <tableColumn id="18" xr3:uid="{A2826505-190A-4FED-8DA4-C03F8C9FF3F3}" uniqueName="18" name="author" queryTableFieldId="18" dataDxfId="136"/>
+    <tableColumn id="2" xr3:uid="{5DCCBB1E-D51F-4A0D-88EA-708103469CAF}" uniqueName="2" name="year" queryTableFieldId="2" dataDxfId="135"/>
+    <tableColumn id="3" xr3:uid="{6DC2321A-EBF3-4A2F-88E3-4B73262A82B8}" uniqueName="3" name="doi" queryTableFieldId="3" dataDxfId="134"/>
+    <tableColumn id="4" xr3:uid="{E980E7C7-406F-4054-87FB-C887DB4B2053}" uniqueName="4" name="url" queryTableFieldId="4" dataDxfId="133"/>
+    <tableColumn id="5" xr3:uid="{34B81B81-EF76-4B54-9237-7AE334AE5578}" uniqueName="5" name="QE parsifal" queryTableFieldId="5" dataDxfId="132"/>
+    <tableColumn id="6" xr3:uid="{594389FB-04A3-4161-B257-EB1DCD730101}" uniqueName="6" name="QE1: related" queryTableFieldId="6" dataDxfId="131"/>
+    <tableColumn id="7" xr3:uid="{0BA238F0-F4F9-4FFE-86B0-8A756146C8D8}" uniqueName="7" name="QE2: method" queryTableFieldId="7" dataDxfId="130"/>
+    <tableColumn id="8" xr3:uid="{C0EB6FEC-D203-4F01-B584-34FE796F2635}" uniqueName="8" name="QE3: l+m" queryTableFieldId="8" dataDxfId="129"/>
+    <tableColumn id="9" xr3:uid="{02418B78-D38A-4642-9393-8AE6F8A5608E}" uniqueName="9" name="QE4: hw+sw" queryTableFieldId="9" dataDxfId="128"/>
+    <tableColumn id="10" xr3:uid="{936B3ED9-F496-4CA5-B86E-E7BA2F308011}" uniqueName="10" name="QE5: long" queryTableFieldId="10" dataDxfId="127"/>
+    <tableColumn id="11" xr3:uid="{76A8C7B4-55B1-4FEB-86A4-19383EA76E7C}" uniqueName="11" name="QE6: others" queryTableFieldId="11" dataDxfId="126"/>
+    <tableColumn id="12" xr3:uid="{1C2CDAEC-857E-46D9-9B69-F4223179257E}" uniqueName="12" name="QE7: public" queryTableFieldId="12" dataDxfId="125"/>
+    <tableColumn id="13" xr3:uid="{4F68A5A7-4AA7-4BBE-93D6-B0B04FD21540}" uniqueName="13" name="QE8: results" queryTableFieldId="13" dataDxfId="124"/>
+    <tableColumn id="14" xr3:uid="{53191D3F-4AC6-4545-B9D6-5191F2222E34}" uniqueName="14" name="QE score" queryTableFieldId="14" dataDxfId="123"/>
+    <tableColumn id="15" xr3:uid="{B1CE6676-AE3F-4BB8-8DC2-32E78F35A19D}" uniqueName="15" name="QE R1:_x000a_QE2/3/5/8" queryTableFieldId="15" dataDxfId="122"/>
+    <tableColumn id="16" xr3:uid="{6AEE4540-681E-42C3-8C64-F84A057E3B2D}" uniqueName="16" name="QE R2:_x000a_cut-off" queryTableFieldId="16" dataDxfId="121"/>
+    <tableColumn id="17" xr3:uid="{8F38DD26-0C87-4DBC-83F8-E3801205D195}" uniqueName="17" name="include?" queryTableFieldId="17" dataDxfId="120"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E3013788-DB09-47C2-A9CD-FE9ABB49D6DA}" name="Table3" displayName="Table3" ref="A1:C25" totalsRowShown="0" headerRowDxfId="126" dataDxfId="125">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{E3013788-DB09-47C2-A9CD-FE9ABB49D6DA}" name="Table3" displayName="Table3" ref="A1:C25" totalsRowShown="0" headerRowDxfId="119" dataDxfId="118">
   <autoFilter ref="A1:C25" xr:uid="{E3013788-DB09-47C2-A9CD-FE9ABB49D6DA}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{E8DC3F13-CC10-4C9A-9911-494D202F9742}" name="index" dataDxfId="124"/>
-    <tableColumn id="2" xr3:uid="{77B0CBB2-98BB-4D99-9163-6271C12647F0}" name="name" dataDxfId="123"/>
-    <tableColumn id="3" xr3:uid="{6B4940E6-8CA7-4E9F-8565-744E144AAF95}" name="details" dataDxfId="122"/>
+    <tableColumn id="1" xr3:uid="{E8DC3F13-CC10-4C9A-9911-494D202F9742}" name="index" dataDxfId="117"/>
+    <tableColumn id="2" xr3:uid="{77B0CBB2-98BB-4D99-9163-6271C12647F0}" name="name" dataDxfId="116"/>
+    <tableColumn id="3" xr3:uid="{6B4940E6-8CA7-4E9F-8565-744E144AAF95}" name="details" dataDxfId="115"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8932CFF7-06FA-420C-81D9-E132C1C847C7}" name="Table4" displayName="Table4" ref="A1:AG177" totalsRowShown="0" headerRowDxfId="121" dataDxfId="120">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8932CFF7-06FA-420C-81D9-E132C1C847C7}" name="Table4" displayName="Table4" ref="A1:AG177" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
   <autoFilter ref="A1:AG177" xr:uid="{8932CFF7-06FA-420C-81D9-E132C1C847C7}"/>
   <tableColumns count="33">
-    <tableColumn id="1" xr3:uid="{5A021834-AF56-418C-B49D-931DD19031CF}" name="title" dataDxfId="119"/>
-    <tableColumn id="30" xr3:uid="{55198485-9B68-4A64-91CA-0B7D5B2CC8A9}" name="author" dataDxfId="118"/>
-    <tableColumn id="2" xr3:uid="{67237C35-097E-4A69-9C6D-E1E784A90835}" name="year" dataDxfId="117"/>
-    <tableColumn id="3" xr3:uid="{750641A9-C68B-491F-AE03-958E2AC8D238}" name="doi" dataDxfId="116"/>
-    <tableColumn id="4" xr3:uid="{A68300A1-F084-47DB-B359-DF766A89AFB6}" name="url" dataDxfId="115"/>
-    <tableColumn id="5" xr3:uid="{E2F101D1-F116-4726-8392-1AF66DE86887}" name="DE1: name" dataDxfId="114"/>
-    <tableColumn id="6" xr3:uid="{D7854BBF-EC4B-45DA-BC88-83C83410C497}" name="DE2: extended version" dataDxfId="113"/>
-    <tableColumn id="7" xr3:uid="{3064C940-1415-4AE4-B6C5-EADCB2ED396F}" name="DE3: long-term" dataDxfId="112"/>
-    <tableColumn id="8" xr3:uid="{8056651C-64E4-4B65-AADC-B44B0C1F6A8D}" name="DE4: local+map" dataDxfId="111"/>
-    <tableColumn id="9" xr3:uid="{CD02B66A-90D5-45A9-AEEE-A6C3F811BC13}" name="DE5: localizer" dataDxfId="110"/>
-    <tableColumn id="10" xr3:uid="{E690E1FB-61A7-4F4A-AB5F-F7AB2B8BD32F}" name="DE6: map" dataDxfId="109"/>
-    <tableColumn id="11" xr3:uid="{2E914CA6-6746-475D-8023-EE867796C757}" name="DE7: active SLAM" dataDxfId="108"/>
-    <tableColumn id="12" xr3:uid="{814C3957-94F7-4B0A-BB19-297ABB920E4D}" name="DE8: SPLAM" dataDxfId="107"/>
-    <tableColumn id="13" xr3:uid="{92553259-C425-4B43-9F38-E915810D111D}" name="DE9: VT&amp;R" dataDxfId="106"/>
-    <tableColumn id="14" xr3:uid="{D8E30307-DAC4-4B41-8FAA-94957323760E}" name="DE10: multi-robot" dataDxfId="105"/>
-    <tableColumn id="15" xr3:uid="{FC8BB1D5-EBDF-472A-B7C7-866660550E67}" name="DE11: prior" dataDxfId="104"/>
-    <tableColumn id="16" xr3:uid="{94AFD69D-9442-4084-BF02-0205A4948C1D}" name="DE12: learning" dataDxfId="103"/>
-    <tableColumn id="17" xr3:uid="{D4C5DE7C-1294-4DF2-8DB5-9A9A0DBF367C}" name="DE13: computation" dataDxfId="102"/>
-    <tableColumn id="18" xr3:uid="{6C6FA01A-F09F-4486-96B3-2CB9A89E9053}" name="DE14: online/offline" dataDxfId="101"/>
-    <tableColumn id="19" xr3:uid="{04BF6F1C-032D-4AD6-91FD-90E385C45303}" name="DE15: environ" dataDxfId="100"/>
-    <tableColumn id="20" xr3:uid="{AE877328-5063-4B45-B8A9-D7F8A6788CE9}" name="DE16: domain" dataDxfId="99"/>
-    <tableColumn id="21" xr3:uid="{6837EAEA-FB13-49FC-BF3B-129500AF30D3}" name="DE17: sensor" dataDxfId="98"/>
-    <tableColumn id="22" xr3:uid="{83BE1EDE-FF47-430D-9298-E9FACC31A6A2}" name="DE18: error eval" dataDxfId="97"/>
-    <tableColumn id="23" xr3:uid="{B6FD116A-6272-46CF-9303-F3062F09A0A6}" name="DE19: compute eval" dataDxfId="96"/>
-    <tableColumn id="24" xr3:uid="{A6B4F75D-8075-47FC-A5E5-FF00B7D8A62E}" name="DE20: gt data" dataDxfId="95"/>
-    <tableColumn id="25" xr3:uid="{72E6FC33-4713-4C64-9835-BB741F784A57}" name="DE21: repo link" dataDxfId="94"/>
-    <tableColumn id="26" xr3:uid="{0DB879B0-4E27-4D88-B9E3-57E8C16B973F}" name="DE22: datasets" dataDxfId="93"/>
-    <tableColumn id="27" xr3:uid="{E5BCF58F-753A-4905-8954-99DB8934DC06}" name="DE23: distance" dataDxfId="92"/>
-    <tableColumn id="28" xr3:uid="{8CA9233F-DA7D-4B60-9B88-7C126BDFB31F}" name="DE24: time" dataDxfId="91"/>
-    <tableColumn id="32" xr3:uid="{38CE948C-EF95-4129-B879-313C625708AD}" name="Notes" dataDxfId="90"/>
-    <tableColumn id="33" xr3:uid="{D1C39509-F985-49D7-9D26-F3DDFBAE5B9F}" name="all data?" dataDxfId="89">
+    <tableColumn id="1" xr3:uid="{5A021834-AF56-418C-B49D-931DD19031CF}" name="title" dataDxfId="32"/>
+    <tableColumn id="30" xr3:uid="{55198485-9B68-4A64-91CA-0B7D5B2CC8A9}" name="author" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{67237C35-097E-4A69-9C6D-E1E784A90835}" name="year" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{750641A9-C68B-491F-AE03-958E2AC8D238}" name="doi" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{A68300A1-F084-47DB-B359-DF766A89AFB6}" name="url" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{E2F101D1-F116-4726-8392-1AF66DE86887}" name="DE1: name" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{D7854BBF-EC4B-45DA-BC88-83C83410C497}" name="DE2: extended version" dataDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{3064C940-1415-4AE4-B6C5-EADCB2ED396F}" name="DE3: long-term" dataDxfId="25"/>
+    <tableColumn id="8" xr3:uid="{8056651C-64E4-4B65-AADC-B44B0C1F6A8D}" name="DE4: local+map" dataDxfId="24"/>
+    <tableColumn id="9" xr3:uid="{CD02B66A-90D5-45A9-AEEE-A6C3F811BC13}" name="DE5: localizer" dataDxfId="23"/>
+    <tableColumn id="10" xr3:uid="{E690E1FB-61A7-4F4A-AB5F-F7AB2B8BD32F}" name="DE6: map" dataDxfId="22"/>
+    <tableColumn id="11" xr3:uid="{2E914CA6-6746-475D-8023-EE867796C757}" name="DE7: active SLAM" dataDxfId="21"/>
+    <tableColumn id="12" xr3:uid="{814C3957-94F7-4B0A-BB19-297ABB920E4D}" name="DE8: SPLAM" dataDxfId="20"/>
+    <tableColumn id="13" xr3:uid="{92553259-C425-4B43-9F38-E915810D111D}" name="DE9: VT&amp;R" dataDxfId="19"/>
+    <tableColumn id="14" xr3:uid="{D8E30307-DAC4-4B41-8FAA-94957323760E}" name="DE10: multi-robot" dataDxfId="18"/>
+    <tableColumn id="15" xr3:uid="{FC8BB1D5-EBDF-472A-B7C7-866660550E67}" name="DE11: prior" dataDxfId="17"/>
+    <tableColumn id="16" xr3:uid="{94AFD69D-9442-4084-BF02-0205A4948C1D}" name="DE12: learning" dataDxfId="16"/>
+    <tableColumn id="17" xr3:uid="{D4C5DE7C-1294-4DF2-8DB5-9A9A0DBF367C}" name="DE13: computation" dataDxfId="15"/>
+    <tableColumn id="18" xr3:uid="{6C6FA01A-F09F-4486-96B3-2CB9A89E9053}" name="DE14: online/offline" dataDxfId="14"/>
+    <tableColumn id="19" xr3:uid="{04BF6F1C-032D-4AD6-91FD-90E385C45303}" name="DE15: environ" dataDxfId="13"/>
+    <tableColumn id="20" xr3:uid="{AE877328-5063-4B45-B8A9-D7F8A6788CE9}" name="DE16: domain" dataDxfId="12"/>
+    <tableColumn id="21" xr3:uid="{6837EAEA-FB13-49FC-BF3B-129500AF30D3}" name="DE17: sensor" dataDxfId="11"/>
+    <tableColumn id="22" xr3:uid="{83BE1EDE-FF47-430D-9298-E9FACC31A6A2}" name="DE18: error eval" dataDxfId="10"/>
+    <tableColumn id="23" xr3:uid="{B6FD116A-6272-46CF-9303-F3062F09A0A6}" name="DE19: compute eval" dataDxfId="9"/>
+    <tableColumn id="24" xr3:uid="{A6B4F75D-8075-47FC-A5E5-FF00B7D8A62E}" name="DE20: gt data" dataDxfId="8"/>
+    <tableColumn id="25" xr3:uid="{72E6FC33-4713-4C64-9835-BB741F784A57}" name="DE21: repo link" dataDxfId="7"/>
+    <tableColumn id="26" xr3:uid="{0DB879B0-4E27-4D88-B9E3-57E8C16B973F}" name="DE22: datasets" dataDxfId="6"/>
+    <tableColumn id="27" xr3:uid="{E5BCF58F-753A-4905-8954-99DB8934DC06}" name="DE23: distance" dataDxfId="5"/>
+    <tableColumn id="28" xr3:uid="{8CA9233F-DA7D-4B60-9B88-7C126BDFB31F}" name="DE24: time" dataDxfId="4"/>
+    <tableColumn id="32" xr3:uid="{38CE948C-EF95-4129-B879-313C625708AD}" name="Notes" dataDxfId="3"/>
+    <tableColumn id="33" xr3:uid="{D1C39509-F985-49D7-9D26-F3DDFBAE5B9F}" name="all data?" dataDxfId="2">
       <calculatedColumnFormula>NOT(OR(ISBLANK(Table4[[#This Row],[DE1: name]]),ISBLANK(Table4[[#This Row],[DE2: extended version]]),ISBLANK(Table4[[#This Row],[DE3: long-term]]),ISBLANK(Table4[[#This Row],[DE4: local+map]]),ISBLANK(Table4[[#This Row],[DE5: localizer]]),ISBLANK(Table4[[#This Row],[DE6: map]]),ISBLANK(Table4[[#This Row],[DE7: active SLAM]]),ISBLANK(Table4[[#This Row],[DE8: SPLAM]]),ISBLANK(Table4[[#This Row],[DE9: VT&amp;R]]),ISBLANK(Table4[[#This Row],[DE10: multi-robot]]),ISBLANK(Table4[[#This Row],[DE11: prior]]),ISBLANK(Table4[[#This Row],[DE12: learning]]),ISBLANK(Table4[[#This Row],[DE13: computation]]),ISBLANK(Table4[[#This Row],[DE14: online/offline]]),ISBLANK(Table4[[#This Row],[DE15: environ]]),ISBLANK(Table4[[#This Row],[DE16: domain]]),ISBLANK(Table4[[#This Row],[DE17: sensor]]),ISBLANK(Table4[[#This Row],[DE18: error eval]]),ISBLANK(Table4[[#This Row],[DE19: compute eval]]),ISBLANK(Table4[[#This Row],[DE20: gt data]]),ISBLANK(Table4[[#This Row],[DE21: repo link]]),ISBLANK(Table4[[#This Row],[DE22: datasets]]),ISBLANK(Table4[[#This Row],[DE23: distance]]),ISBLANK(Table4[[#This Row],[DE24: time]])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{19DD9777-F0DA-4D9E-BEE4-7E22E05AA4B7}" name="data ok?" dataDxfId="88">
+    <tableColumn id="29" xr3:uid="{19DD9777-F0DA-4D9E-BEE4-7E22E05AA4B7}" name="data ok?" dataDxfId="1">
       <calculatedColumnFormula>AND(Table4[[#This Row],[all data?]],NOT(OR(Table4[[#This Row],[DE1: name]]="?",Table4[[#This Row],[DE2: extended version]]="?",Table4[[#This Row],[DE3: long-term]]="?",Table4[[#This Row],[DE4: local+map]]="?",Table4[[#This Row],[DE5: localizer]]="?",Table4[[#This Row],[DE6: map]]="?",Table4[[#This Row],[DE7: active SLAM]]="?",Table4[[#This Row],[DE8: SPLAM]]="?",Table4[[#This Row],[DE9: VT&amp;R]]="?",Table4[[#This Row],[DE10: multi-robot]]="?",Table4[[#This Row],[DE11: prior]]="?",Table4[[#This Row],[DE12: learning]]="?",Table4[[#This Row],[DE13: computation]]="?",Table4[[#This Row],[DE14: online/offline]]="?",Table4[[#This Row],[DE15: environ]]="?",Table4[[#This Row],[DE16: domain]]="?",Table4[[#This Row],[DE17: sensor]]="?",Table4[[#This Row],[DE18: error eval]]="?",Table4[[#This Row],[DE19: compute eval]]="?",Table4[[#This Row],[DE20: gt data]]="?",Table4[[#This Row],[DE21: repo link]]="?",Table4[[#This Row],[DE22: datasets]]="?",Table4[[#This Row],[DE23: distance]]="?",Table4[[#This Row],[DE24: time]]="?")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="31" xr3:uid="{EC011506-2A23-42EF-ADBF-DD3FB87710B3}" name="delete?" dataDxfId="87"/>
+    <tableColumn id="31" xr3:uid="{EC011506-2A23-42EF-ADBF-DD3FB87710B3}" name="delete?" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -35580,31 +35580,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F3:F412">
-    <cfRule type="expression" dxfId="86" priority="1">
+    <cfRule type="expression" dxfId="146" priority="1">
       <formula>$F3=$O3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:N412">
-    <cfRule type="cellIs" dxfId="85" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="5" operator="equal">
       <formula>"full"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="6" operator="equal">
       <formula>"partial"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="7" operator="equal">
       <formula>"none"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O3:R412">
-    <cfRule type="expression" dxfId="82" priority="3">
+    <cfRule type="expression" dxfId="142" priority="3">
       <formula>$R3="yes"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="81" priority="4">
+    <cfRule type="expression" dxfId="141" priority="4">
       <formula>$R3="no"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:R412">
-    <cfRule type="expression" dxfId="80" priority="2">
+    <cfRule type="expression" dxfId="140" priority="2">
       <formula>$F3&lt;&gt;$O3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -52537,322 +52537,322 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <conditionalFormatting sqref="F14:Q14 S14:AF14 F2:AF13 F17:R17 T17:AF17 F18:AF18 F19 Y19:AF19 H19:W19 F20:H21 J20:AF21 AB22:AF22 F22:Z22 F23:AF23 F24:Z26 AB24:AF26 F27:AF29 F31:AF31 F30:S30 U30:AF30 F32:Z32 AB32:AF32 F41:AA41 AC41:AF41 F33:AF40 F42:AF45 AD46:AF46 F47 H47:AF47 F83:S83 U83:AF83 F52:H52 J52:AF52 F53:Z53 AB53:AF53 AE56:AF56 F56:AC56 F63 H63:AF63 F72:S72 U72:AF72 AC85:AF85 F85:AA85 F64:AF68 F69:Q69 S69:AF69 F70:AF70 K71:AF71 F71:I71 F84:AF84 F73:AF75 F77:AF82 L76:AF76 F76:J76 F86:AF89 AA90:AF90 F90:Y90 AB98:AF98 I99:AF99 F91:AF95 F96:G99 I96:AF97 I98:X98 F100:AF104 F105:H105 J105:AF105 F106:Q106 S106:AF106 F107:AF108 F109:G109 W109:AF109 F110:AF110 F111:H111 J111:AF111 Y112:AF112 F112:W112 AD113:AF113 F113:AB113 AA129:AF129 F129:Y129 F135:V135 X135:AF135 F143 H143:AF143 F148:T148 V148:AF148 U168:AF168 F168:Q168 S168 F15:AF16 F48:AF51 F54:AF55 F57:AF62 F114:AF128 F130:AF134 F136:AF142 F144:AF147 F149:AF167 F169:AF177">
-    <cfRule type="cellIs" dxfId="79" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="26" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="27" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:E177 AF2:AF177">
-    <cfRule type="expression" dxfId="77" priority="25">
+    <cfRule type="expression" dxfId="112" priority="25">
       <formula>SEARCH("yes",$AG2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:E177">
-    <cfRule type="expression" dxfId="76" priority="30">
+    <cfRule type="expression" dxfId="111" priority="30">
       <formula>$AF2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="75" priority="32">
+    <cfRule type="expression" dxfId="110" priority="32">
       <formula>AND(NOT($AF2),$AE2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="33">
+    <cfRule type="expression" dxfId="109" priority="33">
       <formula>NOT($AF2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE2:AF25">
-    <cfRule type="expression" dxfId="73" priority="31">
+    <cfRule type="expression" dxfId="108" priority="31">
       <formula>AE2</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="34">
+    <cfRule type="expression" dxfId="107" priority="34">
       <formula>NOT(BH2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19">
-    <cfRule type="cellIs" dxfId="71" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="23" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="24" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T30">
-    <cfRule type="cellIs" dxfId="69" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="21" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="22" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F46:Z46 AB46:AC46">
-    <cfRule type="cellIs" dxfId="67" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="19" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="20" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G47">
-    <cfRule type="cellIs" dxfId="65" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="17" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="18" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I52">
-    <cfRule type="cellIs" dxfId="63" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="15" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="16" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD56">
-    <cfRule type="cellIs" dxfId="61" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="13" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="14" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G63">
-    <cfRule type="cellIs" dxfId="59" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="11" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="12" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y98:AA98">
-    <cfRule type="cellIs" dxfId="57" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="9" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="10" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H109:Q109 S109:V109">
-    <cfRule type="cellIs" dxfId="55" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="7" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="8" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC113">
-    <cfRule type="cellIs" dxfId="53" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="5" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="6" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z129">
-    <cfRule type="cellIs" dxfId="51" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="3" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="4" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G143">
-    <cfRule type="cellIs" dxfId="49" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="1" operator="equal">
       <formula>"?"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="2" operator="equal">
       <formula>"-"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE26:AF48">
-    <cfRule type="expression" dxfId="47" priority="47">
+    <cfRule type="expression" dxfId="82" priority="47">
       <formula>AE26</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="48">
+    <cfRule type="expression" dxfId="81" priority="48">
       <formula>NOT(BH28)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE49:AF53">
-    <cfRule type="expression" dxfId="45" priority="65">
+    <cfRule type="expression" dxfId="80" priority="65">
       <formula>AE49</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="66">
+    <cfRule type="expression" dxfId="79" priority="66">
       <formula>NOT(BH52)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE54:AF59">
-    <cfRule type="expression" dxfId="43" priority="81">
+    <cfRule type="expression" dxfId="78" priority="81">
       <formula>AE54</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="82">
+    <cfRule type="expression" dxfId="77" priority="82">
       <formula>NOT(BH58)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE60:AF60">
-    <cfRule type="expression" dxfId="41" priority="99">
+    <cfRule type="expression" dxfId="76" priority="99">
       <formula>AE60</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="100">
+    <cfRule type="expression" dxfId="75" priority="100">
       <formula>NOT(BH65)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE61:AF95">
-    <cfRule type="expression" dxfId="39" priority="117">
+    <cfRule type="expression" dxfId="74" priority="117">
       <formula>AE61</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="118">
+    <cfRule type="expression" dxfId="73" priority="118">
       <formula>NOT(BH67)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE96:AF110">
-    <cfRule type="expression" dxfId="37" priority="131">
+    <cfRule type="expression" dxfId="72" priority="131">
       <formula>AE96</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="132">
+    <cfRule type="expression" dxfId="71" priority="132">
       <formula>NOT(BH104)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE111:AF118">
-    <cfRule type="expression" dxfId="35" priority="145">
+    <cfRule type="expression" dxfId="70" priority="145">
       <formula>AE111</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="146">
+    <cfRule type="expression" dxfId="69" priority="146">
       <formula>NOT(BH120)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE119:AF121">
-    <cfRule type="expression" dxfId="33" priority="163">
+    <cfRule type="expression" dxfId="68" priority="163">
       <formula>AE119</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="164">
+    <cfRule type="expression" dxfId="67" priority="164">
       <formula>NOT(BH129)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE122:AF124">
-    <cfRule type="expression" dxfId="31" priority="181">
+    <cfRule type="expression" dxfId="66" priority="181">
       <formula>AE122</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="182">
+    <cfRule type="expression" dxfId="65" priority="182">
       <formula>NOT(BH133)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE125:AF126">
-    <cfRule type="expression" dxfId="29" priority="199">
+    <cfRule type="expression" dxfId="64" priority="199">
       <formula>AE125</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="200">
+    <cfRule type="expression" dxfId="63" priority="200">
       <formula>NOT(BH138)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE127:AF128">
-    <cfRule type="expression" dxfId="27" priority="217">
+    <cfRule type="expression" dxfId="62" priority="217">
       <formula>AE127</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="218">
+    <cfRule type="expression" dxfId="61" priority="218">
       <formula>NOT(BH142)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE129:AF130">
-    <cfRule type="expression" dxfId="25" priority="231">
+    <cfRule type="expression" dxfId="60" priority="231">
       <formula>AE129</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="232">
+    <cfRule type="expression" dxfId="59" priority="232">
       <formula>NOT(BH145)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE131:AF136">
-    <cfRule type="expression" dxfId="23" priority="249">
+    <cfRule type="expression" dxfId="58" priority="249">
       <formula>AE131</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="250">
+    <cfRule type="expression" dxfId="57" priority="250">
       <formula>NOT(BH148)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE137:AF138">
-    <cfRule type="expression" dxfId="21" priority="267">
+    <cfRule type="expression" dxfId="56" priority="267">
       <formula>AE137</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="268">
+    <cfRule type="expression" dxfId="55" priority="268">
       <formula>NOT(BH155)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE139:AF143">
-    <cfRule type="expression" dxfId="19" priority="285">
+    <cfRule type="expression" dxfId="54" priority="285">
       <formula>AE139</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="286">
+    <cfRule type="expression" dxfId="53" priority="286">
       <formula>NOT(BH158)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE145:AF151">
-    <cfRule type="expression" dxfId="17" priority="303">
+    <cfRule type="expression" dxfId="52" priority="303">
       <formula>AE145</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="304">
+    <cfRule type="expression" dxfId="51" priority="304">
       <formula>NOT(BH167)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE144:AF144">
-    <cfRule type="expression" dxfId="15" priority="319">
+    <cfRule type="expression" dxfId="50" priority="319">
       <formula>AE144</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="320">
+    <cfRule type="expression" dxfId="49" priority="320">
       <formula>NOT(BH164)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE152:AF154">
-    <cfRule type="expression" dxfId="13" priority="337">
+    <cfRule type="expression" dxfId="48" priority="337">
       <formula>AE152</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="338">
+    <cfRule type="expression" dxfId="47" priority="338">
       <formula>NOT(BH175)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE155:AF155">
-    <cfRule type="expression" dxfId="11" priority="355">
+    <cfRule type="expression" dxfId="46" priority="355">
       <formula>AE155</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="356">
+    <cfRule type="expression" dxfId="45" priority="356">
       <formula>NOT(BH179)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE156:AF162">
-    <cfRule type="expression" dxfId="9" priority="373">
+    <cfRule type="expression" dxfId="44" priority="373">
       <formula>AE156</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="374">
+    <cfRule type="expression" dxfId="43" priority="374">
       <formula>NOT(BH181)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE163:AF168">
-    <cfRule type="expression" dxfId="7" priority="391">
+    <cfRule type="expression" dxfId="42" priority="391">
       <formula>AE163</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="392">
+    <cfRule type="expression" dxfId="41" priority="392">
       <formula>NOT(BH190)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE169:AF173">
-    <cfRule type="expression" dxfId="5" priority="407">
+    <cfRule type="expression" dxfId="40" priority="407">
       <formula>AE169</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="408">
+    <cfRule type="expression" dxfId="39" priority="408">
       <formula>NOT(BH197)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE174:AF174">
-    <cfRule type="expression" dxfId="3" priority="425">
+    <cfRule type="expression" dxfId="38" priority="425">
       <formula>AE174</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="426">
+    <cfRule type="expression" dxfId="37" priority="426">
       <formula>NOT(BH205)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE175:AF177">
-    <cfRule type="expression" dxfId="1" priority="443">
+    <cfRule type="expression" dxfId="36" priority="443">
       <formula>AE175</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="444">
+    <cfRule type="expression" dxfId="35" priority="444">
       <formula>NOT(BH207)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Results initial template for overview section in article
</commit_message>
<xml_diff>
--- a/data/methodology/data-extraction/data.xlsx
+++ b/data/methodology/data-extraction/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sousa\Dev\slr-ltlm-mr\data\methodology\data-extraction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE739FF-839A-4747-BE76-51BB62A44C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523CED3D-FF42-4E95-8FE6-88806B2D275D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3312" yWindow="3312" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Quality Evaluation Scores" sheetId="2" r:id="rId1"/>
@@ -12221,6 +12221,8 @@
   <autoFilter ref="A1:AG176" xr:uid="{8932CFF7-06FA-420C-81D9-E132C1C847C7}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AG176">
     <sortCondition sortBy="cellColor" ref="A2:A176" dxfId="33"/>
+    <sortCondition ref="C2:C176"/>
+    <sortCondition ref="A2:A176"/>
   </sortState>
   <tableColumns count="33">
     <tableColumn id="1" xr3:uid="{5A021834-AF56-418C-B49D-931DD19031CF}" name="title" dataDxfId="32"/>
@@ -50627,37 +50629,37 @@
     </row>
     <row r="148" spans="1:33" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A148" s="5" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B148" s="3" t="s">
         <v>1587</v>
       </c>
       <c r="C148" s="3">
-        <v>2010</v>
+        <v>2009</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E148" s="4" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="F148" s="5" t="s">
         <v>1342</v>
       </c>
       <c r="G148" s="5" t="s">
-        <v>1448</v>
+        <v>1342</v>
       </c>
       <c r="H148" s="5" t="s">
-        <v>1449</v>
+        <v>1406</v>
       </c>
       <c r="I148" s="5" t="s">
-        <v>2053</v>
+        <v>2051</v>
       </c>
       <c r="J148" s="5" t="s">
-        <v>1447</v>
+        <v>1343</v>
       </c>
       <c r="K148" s="5" t="s">
-        <v>1446</v>
+        <v>1407</v>
       </c>
       <c r="L148" s="5" t="s">
         <v>655</v>
@@ -50690,13 +50692,13 @@
         <v>1353</v>
       </c>
       <c r="V148" s="5" t="s">
-        <v>1445</v>
+        <v>1371</v>
       </c>
       <c r="W148" s="5" t="s">
-        <v>1453</v>
+        <v>1412</v>
       </c>
       <c r="X148" s="5" t="s">
-        <v>1342</v>
+        <v>1410</v>
       </c>
       <c r="Y148" s="5" t="s">
         <v>1409</v>
@@ -50708,13 +50710,13 @@
         <v>1342</v>
       </c>
       <c r="AB148" s="5" t="s">
-        <v>1452</v>
+        <v>1408</v>
       </c>
       <c r="AC148" s="5" t="s">
         <v>1342</v>
       </c>
       <c r="AD148" s="5" t="s">
-        <v>1450</v>
+        <v>1342</v>
       </c>
       <c r="AE148" s="5" t="b">
         <f>NOT(OR(ISBLANK(Table4[[#This Row],[DE1: name]]),ISBLANK(Table4[[#This Row],[DE2: extended version]]),ISBLANK(Table4[[#This Row],[DE3: long-term]]),ISBLANK(Table4[[#This Row],[DE4: local+map]]),ISBLANK(Table4[[#This Row],[DE5: localizer]]),ISBLANK(Table4[[#This Row],[DE6: map]]),ISBLANK(Table4[[#This Row],[DE7: active SLAM]]),ISBLANK(Table4[[#This Row],[DE8: SPLAM]]),ISBLANK(Table4[[#This Row],[DE9: VT&amp;R]]),ISBLANK(Table4[[#This Row],[DE10: multi-robot]]),ISBLANK(Table4[[#This Row],[DE11: prior]]),ISBLANK(Table4[[#This Row],[DE12: learning]]),ISBLANK(Table4[[#This Row],[DE13: computation]]),ISBLANK(Table4[[#This Row],[DE14: online/offline]]),ISBLANK(Table4[[#This Row],[DE15: environ]]),ISBLANK(Table4[[#This Row],[DE16: domain]]),ISBLANK(Table4[[#This Row],[DE17: sensor]]),ISBLANK(Table4[[#This Row],[DE18: error eval]]),ISBLANK(Table4[[#This Row],[DE19: compute eval]]),ISBLANK(Table4[[#This Row],[DE20: gt data]]),ISBLANK(Table4[[#This Row],[DE21: repo link]]),ISBLANK(Table4[[#This Row],[DE22: datasets]]),ISBLANK(Table4[[#This Row],[DE23: distance]]),ISBLANK(Table4[[#This Row],[DE24: time]])))</f>
@@ -50725,42 +50727,42 @@
         <v>1</v>
       </c>
       <c r="AG148" s="5" t="s">
-        <v>1451</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="149" spans="1:33" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A149" s="5" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>1593</v>
+        <v>1587</v>
       </c>
       <c r="C149" s="3">
         <v>2010</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="E149" s="4" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="F149" s="5" t="s">
         <v>1342</v>
       </c>
       <c r="G149" s="5" t="s">
-        <v>1342</v>
+        <v>1448</v>
       </c>
       <c r="H149" s="5" t="s">
-        <v>1475</v>
+        <v>1449</v>
       </c>
       <c r="I149" s="5" t="s">
-        <v>2055</v>
+        <v>2053</v>
       </c>
       <c r="J149" s="5" t="s">
-        <v>1476</v>
+        <v>1447</v>
       </c>
       <c r="K149" s="5" t="s">
-        <v>1474</v>
+        <v>1446</v>
       </c>
       <c r="L149" s="5" t="s">
         <v>655</v>
@@ -50787,22 +50789,22 @@
         <v>1351</v>
       </c>
       <c r="T149" s="5" t="s">
-        <v>1478</v>
+        <v>1352</v>
       </c>
       <c r="U149" s="5" t="s">
         <v>1353</v>
       </c>
       <c r="V149" s="5" t="s">
-        <v>1371</v>
+        <v>1445</v>
       </c>
       <c r="W149" s="5" t="s">
-        <v>1477</v>
+        <v>1453</v>
       </c>
       <c r="X149" s="5" t="s">
         <v>1342</v>
       </c>
       <c r="Y149" s="5" t="s">
-        <v>1342</v>
+        <v>1409</v>
       </c>
       <c r="Z149" s="5" t="s">
         <v>1342</v>
@@ -50811,13 +50813,13 @@
         <v>1342</v>
       </c>
       <c r="AB149" s="5" t="s">
-        <v>1342</v>
+        <v>1452</v>
       </c>
       <c r="AC149" s="5" t="s">
         <v>1342</v>
       </c>
       <c r="AD149" s="5" t="s">
-        <v>1342</v>
+        <v>1450</v>
       </c>
       <c r="AE149" s="5" t="b">
         <f>NOT(OR(ISBLANK(Table4[[#This Row],[DE1: name]]),ISBLANK(Table4[[#This Row],[DE2: extended version]]),ISBLANK(Table4[[#This Row],[DE3: long-term]]),ISBLANK(Table4[[#This Row],[DE4: local+map]]),ISBLANK(Table4[[#This Row],[DE5: localizer]]),ISBLANK(Table4[[#This Row],[DE6: map]]),ISBLANK(Table4[[#This Row],[DE7: active SLAM]]),ISBLANK(Table4[[#This Row],[DE8: SPLAM]]),ISBLANK(Table4[[#This Row],[DE9: VT&amp;R]]),ISBLANK(Table4[[#This Row],[DE10: multi-robot]]),ISBLANK(Table4[[#This Row],[DE11: prior]]),ISBLANK(Table4[[#This Row],[DE12: learning]]),ISBLANK(Table4[[#This Row],[DE13: computation]]),ISBLANK(Table4[[#This Row],[DE14: online/offline]]),ISBLANK(Table4[[#This Row],[DE15: environ]]),ISBLANK(Table4[[#This Row],[DE16: domain]]),ISBLANK(Table4[[#This Row],[DE17: sensor]]),ISBLANK(Table4[[#This Row],[DE18: error eval]]),ISBLANK(Table4[[#This Row],[DE19: compute eval]]),ISBLANK(Table4[[#This Row],[DE20: gt data]]),ISBLANK(Table4[[#This Row],[DE21: repo link]]),ISBLANK(Table4[[#This Row],[DE22: datasets]]),ISBLANK(Table4[[#This Row],[DE23: distance]]),ISBLANK(Table4[[#This Row],[DE24: time]])))</f>
@@ -50833,19 +50835,19 @@
     </row>
     <row r="150" spans="1:33" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A150" s="5" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>1587</v>
+        <v>1593</v>
       </c>
       <c r="C150" s="3">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>38</v>
+        <v>63</v>
       </c>
       <c r="E150" s="4" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="F150" s="5" t="s">
         <v>1342</v>
@@ -50854,16 +50856,16 @@
         <v>1342</v>
       </c>
       <c r="H150" s="5" t="s">
-        <v>1406</v>
+        <v>1475</v>
       </c>
       <c r="I150" s="5" t="s">
-        <v>2051</v>
+        <v>2055</v>
       </c>
       <c r="J150" s="5" t="s">
-        <v>1343</v>
+        <v>1476</v>
       </c>
       <c r="K150" s="5" t="s">
-        <v>1407</v>
+        <v>1474</v>
       </c>
       <c r="L150" s="5" t="s">
         <v>655</v>
@@ -50890,7 +50892,7 @@
         <v>1351</v>
       </c>
       <c r="T150" s="5" t="s">
-        <v>1352</v>
+        <v>1478</v>
       </c>
       <c r="U150" s="5" t="s">
         <v>1353</v>
@@ -50899,13 +50901,13 @@
         <v>1371</v>
       </c>
       <c r="W150" s="5" t="s">
-        <v>1412</v>
+        <v>1477</v>
       </c>
       <c r="X150" s="5" t="s">
-        <v>1410</v>
+        <v>1342</v>
       </c>
       <c r="Y150" s="5" t="s">
-        <v>1409</v>
+        <v>1342</v>
       </c>
       <c r="Z150" s="5" t="s">
         <v>1342</v>
@@ -50914,7 +50916,7 @@
         <v>1342</v>
       </c>
       <c r="AB150" s="5" t="s">
-        <v>1408</v>
+        <v>1342</v>
       </c>
       <c r="AC150" s="5" t="s">
         <v>1342</v>
@@ -50931,7 +50933,7 @@
         <v>1</v>
       </c>
       <c r="AG150" s="5" t="s">
-        <v>1434</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="151" spans="1:33" ht="171.6" x14ac:dyDescent="0.3">
@@ -51037,39 +51039,39 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="152" spans="1:33" ht="132" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:33" ht="184.8" x14ac:dyDescent="0.3">
       <c r="A152" s="5" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>1603</v>
+        <v>1600</v>
       </c>
       <c r="C152" s="3">
         <v>2011</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E152" s="4" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="F152" s="5" t="s">
-        <v>1544</v>
+        <v>1532</v>
       </c>
       <c r="G152" s="5" t="s">
         <v>1342</v>
       </c>
       <c r="H152" s="5" t="s">
-        <v>1554</v>
+        <v>1533</v>
       </c>
       <c r="I152" s="5" t="s">
-        <v>1553</v>
+        <v>1386</v>
       </c>
       <c r="J152" s="5" t="s">
-        <v>1556</v>
+        <v>1535</v>
       </c>
       <c r="K152" s="5" t="s">
-        <v>1555</v>
+        <v>1534</v>
       </c>
       <c r="L152" s="5" t="s">
         <v>655</v>
@@ -51084,19 +51086,19 @@
         <v>655</v>
       </c>
       <c r="P152" s="5" t="s">
-        <v>1493</v>
+        <v>655</v>
       </c>
       <c r="Q152" s="5" t="s">
-        <v>1557</v>
+        <v>655</v>
       </c>
       <c r="R152" s="5" t="s">
         <v>1349</v>
       </c>
       <c r="S152" s="5" t="s">
-        <v>1561</v>
+        <v>1351</v>
       </c>
       <c r="T152" s="5" t="s">
-        <v>1558</v>
+        <v>1399</v>
       </c>
       <c r="U152" s="5" t="s">
         <v>1353</v>
@@ -51108,19 +51110,19 @@
         <v>1536</v>
       </c>
       <c r="X152" s="5" t="s">
-        <v>1342</v>
+        <v>1537</v>
       </c>
       <c r="Y152" s="5" t="s">
         <v>1538</v>
       </c>
       <c r="Z152" s="5" t="s">
-        <v>1342</v>
+        <v>1539</v>
       </c>
       <c r="AA152" s="5" t="s">
-        <v>1559</v>
+        <v>1540</v>
       </c>
       <c r="AB152" s="5" t="s">
-        <v>1560</v>
+        <v>1342</v>
       </c>
       <c r="AC152" s="5" t="s">
         <v>1342</v>
@@ -51137,145 +51139,76 @@
         <v>1</v>
       </c>
       <c r="AG152" s="5" t="s">
-        <v>1434</v>
-      </c>
-    </row>
-    <row r="153" spans="1:33" ht="105.6" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="153" spans="1:33" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A153" s="5" t="s">
-        <v>125</v>
+        <v>89</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>1610</v>
+        <v>1601</v>
       </c>
       <c r="C153" s="3">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E153" s="16" t="s">
-        <v>127</v>
+        <v>90</v>
+      </c>
+      <c r="E153" s="4" t="s">
+        <v>91</v>
       </c>
       <c r="F153" s="5" t="s">
-        <v>1342</v>
+        <v>1545</v>
       </c>
       <c r="G153" s="5" t="s">
-        <v>1342</v>
-      </c>
-      <c r="H153" s="5" t="s">
-        <v>2009</v>
-      </c>
-      <c r="I153" s="5" t="s">
-        <v>1386</v>
-      </c>
-      <c r="J153" s="5" t="s">
-        <v>2014</v>
-      </c>
-      <c r="K153" s="5" t="s">
-        <v>2013</v>
-      </c>
-      <c r="L153" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="M153" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="N153" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="O153" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="P153" s="5" t="s">
-        <v>1493</v>
-      </c>
-      <c r="Q153" s="5" t="s">
-        <v>2010</v>
-      </c>
-      <c r="R153" s="5" t="s">
-        <v>1349</v>
-      </c>
-      <c r="S153" s="5" t="s">
-        <v>1342</v>
-      </c>
-      <c r="T153" s="5" t="s">
-        <v>1399</v>
-      </c>
-      <c r="U153" s="5" t="s">
-        <v>1353</v>
-      </c>
-      <c r="V153" s="5" t="s">
-        <v>1357</v>
-      </c>
-      <c r="W153" s="5" t="s">
-        <v>1536</v>
-      </c>
-      <c r="X153" s="5" t="s">
-        <v>1342</v>
-      </c>
-      <c r="Y153" s="5" t="s">
-        <v>1538</v>
-      </c>
-      <c r="Z153" s="5" t="s">
-        <v>1342</v>
-      </c>
-      <c r="AA153" s="5" t="s">
-        <v>2015</v>
-      </c>
-      <c r="AB153" s="5" t="s">
-        <v>2016</v>
-      </c>
-      <c r="AC153" s="5" t="s">
-        <v>2017</v>
-      </c>
-      <c r="AD153" s="5" t="s">
-        <v>1342</v>
+        <v>1541</v>
       </c>
       <c r="AE153" s="5" t="b">
         <f>NOT(OR(ISBLANK(Table4[[#This Row],[DE1: name]]),ISBLANK(Table4[[#This Row],[DE2: extended version]]),ISBLANK(Table4[[#This Row],[DE3: long-term]]),ISBLANK(Table4[[#This Row],[DE4: local+map]]),ISBLANK(Table4[[#This Row],[DE5: localizer]]),ISBLANK(Table4[[#This Row],[DE6: map]]),ISBLANK(Table4[[#This Row],[DE7: active SLAM]]),ISBLANK(Table4[[#This Row],[DE8: SPLAM]]),ISBLANK(Table4[[#This Row],[DE9: VT&amp;R]]),ISBLANK(Table4[[#This Row],[DE10: multi-robot]]),ISBLANK(Table4[[#This Row],[DE11: prior]]),ISBLANK(Table4[[#This Row],[DE12: learning]]),ISBLANK(Table4[[#This Row],[DE13: computation]]),ISBLANK(Table4[[#This Row],[DE14: online/offline]]),ISBLANK(Table4[[#This Row],[DE15: environ]]),ISBLANK(Table4[[#This Row],[DE16: domain]]),ISBLANK(Table4[[#This Row],[DE17: sensor]]),ISBLANK(Table4[[#This Row],[DE18: error eval]]),ISBLANK(Table4[[#This Row],[DE19: compute eval]]),ISBLANK(Table4[[#This Row],[DE20: gt data]]),ISBLANK(Table4[[#This Row],[DE21: repo link]]),ISBLANK(Table4[[#This Row],[DE22: datasets]]),ISBLANK(Table4[[#This Row],[DE23: distance]]),ISBLANK(Table4[[#This Row],[DE24: time]])))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF153" s="5" t="b">
         <f>AND(Table4[[#This Row],[all data?]],NOT(OR(Table4[[#This Row],[DE1: name]]="?",Table4[[#This Row],[DE2: extended version]]="?",Table4[[#This Row],[DE3: long-term]]="?",Table4[[#This Row],[DE4: local+map]]="?",Table4[[#This Row],[DE5: localizer]]="?",Table4[[#This Row],[DE6: map]]="?",Table4[[#This Row],[DE7: active SLAM]]="?",Table4[[#This Row],[DE8: SPLAM]]="?",Table4[[#This Row],[DE9: VT&amp;R]]="?",Table4[[#This Row],[DE10: multi-robot]]="?",Table4[[#This Row],[DE11: prior]]="?",Table4[[#This Row],[DE12: learning]]="?",Table4[[#This Row],[DE13: computation]]="?",Table4[[#This Row],[DE14: online/offline]]="?",Table4[[#This Row],[DE15: environ]]="?",Table4[[#This Row],[DE16: domain]]="?",Table4[[#This Row],[DE17: sensor]]="?",Table4[[#This Row],[DE18: error eval]]="?",Table4[[#This Row],[DE19: compute eval]]="?",Table4[[#This Row],[DE20: gt data]]="?",Table4[[#This Row],[DE21: repo link]]="?",Table4[[#This Row],[DE22: datasets]]="?",Table4[[#This Row],[DE23: distance]]="?",Table4[[#This Row],[DE24: time]]="?")))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG153" s="5" t="s">
-        <v>1434</v>
-      </c>
-    </row>
-    <row r="154" spans="1:33" ht="184.8" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="154" spans="1:33" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A154" s="5" t="s">
-        <v>152</v>
+        <v>92</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>1619</v>
+        <v>1602</v>
       </c>
       <c r="C154" s="3">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>153</v>
+        <v>93</v>
       </c>
       <c r="E154" s="4" t="s">
-        <v>154</v>
+        <v>94</v>
       </c>
       <c r="F154" s="5" t="s">
-        <v>1342</v>
+        <v>1543</v>
       </c>
       <c r="G154" s="5" t="s">
-        <v>1342</v>
+        <v>1542</v>
       </c>
       <c r="H154" s="5" t="s">
-        <v>2085</v>
+        <v>1547</v>
       </c>
       <c r="I154" s="5" t="s">
-        <v>1342</v>
+        <v>1386</v>
       </c>
       <c r="J154" s="5" t="s">
-        <v>1342</v>
+        <v>1484</v>
       </c>
       <c r="K154" s="5" t="s">
-        <v>2088</v>
+        <v>2012</v>
       </c>
       <c r="L154" s="5" t="s">
         <v>655</v>
@@ -51299,40 +51232,40 @@
         <v>1349</v>
       </c>
       <c r="S154" s="5" t="s">
-        <v>2086</v>
+        <v>1351</v>
       </c>
       <c r="T154" s="5" t="s">
-        <v>1972</v>
+        <v>1548</v>
       </c>
       <c r="U154" s="5" t="s">
         <v>1353</v>
       </c>
       <c r="V154" s="5" t="s">
-        <v>2089</v>
+        <v>1481</v>
       </c>
       <c r="W154" s="5" t="s">
-        <v>2092</v>
+        <v>1550</v>
       </c>
       <c r="X154" s="5" t="s">
-        <v>2093</v>
+        <v>1549</v>
       </c>
       <c r="Y154" s="5" t="s">
-        <v>2087</v>
+        <v>1551</v>
       </c>
       <c r="Z154" s="5" t="s">
-        <v>2094</v>
+        <v>1342</v>
       </c>
       <c r="AA154" s="5" t="s">
-        <v>1342</v>
+        <v>1552</v>
       </c>
       <c r="AB154" s="5" t="s">
-        <v>2091</v>
+        <v>1342</v>
       </c>
       <c r="AC154" s="5" t="s">
-        <v>2090</v>
+        <v>1342</v>
       </c>
       <c r="AD154" s="5" t="s">
-        <v>1342</v>
+        <v>1546</v>
       </c>
       <c r="AE154" s="5" t="b">
         <f>NOT(OR(ISBLANK(Table4[[#This Row],[DE1: name]]),ISBLANK(Table4[[#This Row],[DE2: extended version]]),ISBLANK(Table4[[#This Row],[DE3: long-term]]),ISBLANK(Table4[[#This Row],[DE4: local+map]]),ISBLANK(Table4[[#This Row],[DE5: localizer]]),ISBLANK(Table4[[#This Row],[DE6: map]]),ISBLANK(Table4[[#This Row],[DE7: active SLAM]]),ISBLANK(Table4[[#This Row],[DE8: SPLAM]]),ISBLANK(Table4[[#This Row],[DE9: VT&amp;R]]),ISBLANK(Table4[[#This Row],[DE10: multi-robot]]),ISBLANK(Table4[[#This Row],[DE11: prior]]),ISBLANK(Table4[[#This Row],[DE12: learning]]),ISBLANK(Table4[[#This Row],[DE13: computation]]),ISBLANK(Table4[[#This Row],[DE14: online/offline]]),ISBLANK(Table4[[#This Row],[DE15: environ]]),ISBLANK(Table4[[#This Row],[DE16: domain]]),ISBLANK(Table4[[#This Row],[DE17: sensor]]),ISBLANK(Table4[[#This Row],[DE18: error eval]]),ISBLANK(Table4[[#This Row],[DE19: compute eval]]),ISBLANK(Table4[[#This Row],[DE20: gt data]]),ISBLANK(Table4[[#This Row],[DE21: repo link]]),ISBLANK(Table4[[#This Row],[DE22: datasets]]),ISBLANK(Table4[[#This Row],[DE23: distance]]),ISBLANK(Table4[[#This Row],[DE24: time]])))</f>
@@ -51343,107 +51276,233 @@
         <v>1</v>
       </c>
       <c r="AG154" s="5" t="s">
-        <v>1434</v>
-      </c>
-    </row>
-    <row r="155" spans="1:33" ht="52.8" x14ac:dyDescent="0.3">
+        <v>2001</v>
+      </c>
+    </row>
+    <row r="155" spans="1:33" ht="132" x14ac:dyDescent="0.3">
       <c r="A155" s="5" t="s">
-        <v>158</v>
+        <v>95</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>1607</v>
+        <v>1603</v>
       </c>
       <c r="C155" s="3">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>159</v>
+        <v>96</v>
       </c>
       <c r="E155" s="4" t="s">
-        <v>160</v>
+        <v>97</v>
       </c>
       <c r="F155" s="5" t="s">
-        <v>1968</v>
+        <v>1544</v>
       </c>
       <c r="G155" s="5" t="s">
         <v>1342</v>
       </c>
+      <c r="H155" s="5" t="s">
+        <v>1554</v>
+      </c>
+      <c r="I155" s="5" t="s">
+        <v>1553</v>
+      </c>
+      <c r="J155" s="5" t="s">
+        <v>1556</v>
+      </c>
+      <c r="K155" s="5" t="s">
+        <v>1555</v>
+      </c>
+      <c r="L155" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="M155" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="N155" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="O155" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="P155" s="5" t="s">
+        <v>1493</v>
+      </c>
+      <c r="Q155" s="5" t="s">
+        <v>1557</v>
+      </c>
+      <c r="R155" s="5" t="s">
+        <v>1349</v>
+      </c>
+      <c r="S155" s="5" t="s">
+        <v>1561</v>
+      </c>
+      <c r="T155" s="5" t="s">
+        <v>1558</v>
+      </c>
+      <c r="U155" s="5" t="s">
+        <v>1353</v>
+      </c>
+      <c r="V155" s="5" t="s">
+        <v>1357</v>
+      </c>
+      <c r="W155" s="5" t="s">
+        <v>1536</v>
+      </c>
+      <c r="X155" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="Y155" s="5" t="s">
+        <v>1538</v>
+      </c>
+      <c r="Z155" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="AA155" s="5" t="s">
+        <v>1559</v>
+      </c>
+      <c r="AB155" s="5" t="s">
+        <v>1560</v>
+      </c>
+      <c r="AC155" s="5" t="s">
+        <v>1342</v>
+      </c>
       <c r="AD155" s="5" t="s">
-        <v>2110</v>
+        <v>1342</v>
       </c>
       <c r="AE155" s="5" t="b">
         <f>NOT(OR(ISBLANK(Table4[[#This Row],[DE1: name]]),ISBLANK(Table4[[#This Row],[DE2: extended version]]),ISBLANK(Table4[[#This Row],[DE3: long-term]]),ISBLANK(Table4[[#This Row],[DE4: local+map]]),ISBLANK(Table4[[#This Row],[DE5: localizer]]),ISBLANK(Table4[[#This Row],[DE6: map]]),ISBLANK(Table4[[#This Row],[DE7: active SLAM]]),ISBLANK(Table4[[#This Row],[DE8: SPLAM]]),ISBLANK(Table4[[#This Row],[DE9: VT&amp;R]]),ISBLANK(Table4[[#This Row],[DE10: multi-robot]]),ISBLANK(Table4[[#This Row],[DE11: prior]]),ISBLANK(Table4[[#This Row],[DE12: learning]]),ISBLANK(Table4[[#This Row],[DE13: computation]]),ISBLANK(Table4[[#This Row],[DE14: online/offline]]),ISBLANK(Table4[[#This Row],[DE15: environ]]),ISBLANK(Table4[[#This Row],[DE16: domain]]),ISBLANK(Table4[[#This Row],[DE17: sensor]]),ISBLANK(Table4[[#This Row],[DE18: error eval]]),ISBLANK(Table4[[#This Row],[DE19: compute eval]]),ISBLANK(Table4[[#This Row],[DE20: gt data]]),ISBLANK(Table4[[#This Row],[DE21: repo link]]),ISBLANK(Table4[[#This Row],[DE22: datasets]]),ISBLANK(Table4[[#This Row],[DE23: distance]]),ISBLANK(Table4[[#This Row],[DE24: time]])))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF155" s="5" t="b">
         <f>AND(Table4[[#This Row],[all data?]],NOT(OR(Table4[[#This Row],[DE1: name]]="?",Table4[[#This Row],[DE2: extended version]]="?",Table4[[#This Row],[DE3: long-term]]="?",Table4[[#This Row],[DE4: local+map]]="?",Table4[[#This Row],[DE5: localizer]]="?",Table4[[#This Row],[DE6: map]]="?",Table4[[#This Row],[DE7: active SLAM]]="?",Table4[[#This Row],[DE8: SPLAM]]="?",Table4[[#This Row],[DE9: VT&amp;R]]="?",Table4[[#This Row],[DE10: multi-robot]]="?",Table4[[#This Row],[DE11: prior]]="?",Table4[[#This Row],[DE12: learning]]="?",Table4[[#This Row],[DE13: computation]]="?",Table4[[#This Row],[DE14: online/offline]]="?",Table4[[#This Row],[DE15: environ]]="?",Table4[[#This Row],[DE16: domain]]="?",Table4[[#This Row],[DE17: sensor]]="?",Table4[[#This Row],[DE18: error eval]]="?",Table4[[#This Row],[DE19: compute eval]]="?",Table4[[#This Row],[DE20: gt data]]="?",Table4[[#This Row],[DE21: repo link]]="?",Table4[[#This Row],[DE22: datasets]]="?",Table4[[#This Row],[DE23: distance]]="?",Table4[[#This Row],[DE24: time]]="?")))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG155" s="5" t="s">
         <v>1434</v>
       </c>
     </row>
-    <row r="156" spans="1:33" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:33" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A156" s="5" t="s">
-        <v>161</v>
+        <v>125</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>1607</v>
+        <v>1610</v>
       </c>
       <c r="C156" s="3">
         <v>2013</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="E156" s="4" t="s">
-        <v>163</v>
+        <v>126</v>
+      </c>
+      <c r="E156" s="16" t="s">
+        <v>127</v>
       </c>
       <c r="F156" s="5" t="s">
-        <v>1968</v>
+        <v>1342</v>
       </c>
       <c r="G156" s="5" t="s">
         <v>1342</v>
       </c>
+      <c r="H156" s="5" t="s">
+        <v>2009</v>
+      </c>
+      <c r="I156" s="5" t="s">
+        <v>1386</v>
+      </c>
+      <c r="J156" s="5" t="s">
+        <v>2014</v>
+      </c>
+      <c r="K156" s="5" t="s">
+        <v>2013</v>
+      </c>
+      <c r="L156" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="M156" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="N156" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="O156" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="P156" s="5" t="s">
+        <v>1493</v>
+      </c>
+      <c r="Q156" s="5" t="s">
+        <v>2010</v>
+      </c>
+      <c r="R156" s="5" t="s">
+        <v>1349</v>
+      </c>
+      <c r="S156" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="T156" s="5" t="s">
+        <v>1399</v>
+      </c>
+      <c r="U156" s="5" t="s">
+        <v>1353</v>
+      </c>
+      <c r="V156" s="5" t="s">
+        <v>1357</v>
+      </c>
+      <c r="W156" s="5" t="s">
+        <v>1536</v>
+      </c>
+      <c r="X156" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="Y156" s="5" t="s">
+        <v>1538</v>
+      </c>
+      <c r="Z156" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="AA156" s="5" t="s">
+        <v>2015</v>
+      </c>
+      <c r="AB156" s="5" t="s">
+        <v>2016</v>
+      </c>
+      <c r="AC156" s="5" t="s">
+        <v>2017</v>
+      </c>
       <c r="AD156" s="5" t="s">
-        <v>2110</v>
+        <v>1342</v>
       </c>
       <c r="AE156" s="5" t="b">
         <f>NOT(OR(ISBLANK(Table4[[#This Row],[DE1: name]]),ISBLANK(Table4[[#This Row],[DE2: extended version]]),ISBLANK(Table4[[#This Row],[DE3: long-term]]),ISBLANK(Table4[[#This Row],[DE4: local+map]]),ISBLANK(Table4[[#This Row],[DE5: localizer]]),ISBLANK(Table4[[#This Row],[DE6: map]]),ISBLANK(Table4[[#This Row],[DE7: active SLAM]]),ISBLANK(Table4[[#This Row],[DE8: SPLAM]]),ISBLANK(Table4[[#This Row],[DE9: VT&amp;R]]),ISBLANK(Table4[[#This Row],[DE10: multi-robot]]),ISBLANK(Table4[[#This Row],[DE11: prior]]),ISBLANK(Table4[[#This Row],[DE12: learning]]),ISBLANK(Table4[[#This Row],[DE13: computation]]),ISBLANK(Table4[[#This Row],[DE14: online/offline]]),ISBLANK(Table4[[#This Row],[DE15: environ]]),ISBLANK(Table4[[#This Row],[DE16: domain]]),ISBLANK(Table4[[#This Row],[DE17: sensor]]),ISBLANK(Table4[[#This Row],[DE18: error eval]]),ISBLANK(Table4[[#This Row],[DE19: compute eval]]),ISBLANK(Table4[[#This Row],[DE20: gt data]]),ISBLANK(Table4[[#This Row],[DE21: repo link]]),ISBLANK(Table4[[#This Row],[DE22: datasets]]),ISBLANK(Table4[[#This Row],[DE23: distance]]),ISBLANK(Table4[[#This Row],[DE24: time]])))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF156" s="5" t="b">
         <f>AND(Table4[[#This Row],[all data?]],NOT(OR(Table4[[#This Row],[DE1: name]]="?",Table4[[#This Row],[DE2: extended version]]="?",Table4[[#This Row],[DE3: long-term]]="?",Table4[[#This Row],[DE4: local+map]]="?",Table4[[#This Row],[DE5: localizer]]="?",Table4[[#This Row],[DE6: map]]="?",Table4[[#This Row],[DE7: active SLAM]]="?",Table4[[#This Row],[DE8: SPLAM]]="?",Table4[[#This Row],[DE9: VT&amp;R]]="?",Table4[[#This Row],[DE10: multi-robot]]="?",Table4[[#This Row],[DE11: prior]]="?",Table4[[#This Row],[DE12: learning]]="?",Table4[[#This Row],[DE13: computation]]="?",Table4[[#This Row],[DE14: online/offline]]="?",Table4[[#This Row],[DE15: environ]]="?",Table4[[#This Row],[DE16: domain]]="?",Table4[[#This Row],[DE17: sensor]]="?",Table4[[#This Row],[DE18: error eval]]="?",Table4[[#This Row],[DE19: compute eval]]="?",Table4[[#This Row],[DE20: gt data]]="?",Table4[[#This Row],[DE21: repo link]]="?",Table4[[#This Row],[DE22: datasets]]="?",Table4[[#This Row],[DE23: distance]]="?",Table4[[#This Row],[DE24: time]]="?")))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG156" s="5" t="s">
         <v>1434</v>
       </c>
     </row>
-    <row r="157" spans="1:33" ht="66" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:33" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A157" s="5" t="s">
-        <v>179</v>
+        <v>128</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>1624</v>
+        <v>1611</v>
       </c>
       <c r="C157" s="3">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>180</v>
+        <v>129</v>
       </c>
       <c r="E157" s="4" t="s">
-        <v>181</v>
+        <v>130</v>
       </c>
       <c r="F157" s="5" t="s">
-        <v>2149</v>
-      </c>
-      <c r="G157" s="5" t="s">
-        <v>1342</v>
-      </c>
-      <c r="AD157" s="5" t="s">
-        <v>2150</v>
+        <v>1532</v>
       </c>
       <c r="AE157" s="5" t="b">
         <f>NOT(OR(ISBLANK(Table4[[#This Row],[DE1: name]]),ISBLANK(Table4[[#This Row],[DE2: extended version]]),ISBLANK(Table4[[#This Row],[DE3: long-term]]),ISBLANK(Table4[[#This Row],[DE4: local+map]]),ISBLANK(Table4[[#This Row],[DE5: localizer]]),ISBLANK(Table4[[#This Row],[DE6: map]]),ISBLANK(Table4[[#This Row],[DE7: active SLAM]]),ISBLANK(Table4[[#This Row],[DE8: SPLAM]]),ISBLANK(Table4[[#This Row],[DE9: VT&amp;R]]),ISBLANK(Table4[[#This Row],[DE10: multi-robot]]),ISBLANK(Table4[[#This Row],[DE11: prior]]),ISBLANK(Table4[[#This Row],[DE12: learning]]),ISBLANK(Table4[[#This Row],[DE13: computation]]),ISBLANK(Table4[[#This Row],[DE14: online/offline]]),ISBLANK(Table4[[#This Row],[DE15: environ]]),ISBLANK(Table4[[#This Row],[DE16: domain]]),ISBLANK(Table4[[#This Row],[DE17: sensor]]),ISBLANK(Table4[[#This Row],[DE18: error eval]]),ISBLANK(Table4[[#This Row],[DE19: compute eval]]),ISBLANK(Table4[[#This Row],[DE20: gt data]]),ISBLANK(Table4[[#This Row],[DE21: repo link]]),ISBLANK(Table4[[#This Row],[DE22: datasets]]),ISBLANK(Table4[[#This Row],[DE23: distance]]),ISBLANK(Table4[[#This Row],[DE24: time]])))</f>
@@ -51454,32 +51513,107 @@
         <v>0</v>
       </c>
       <c r="AG157" s="5" t="s">
-        <v>1434</v>
-      </c>
-    </row>
-    <row r="158" spans="1:33" ht="52.8" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="158" spans="1:33" ht="184.8" x14ac:dyDescent="0.3">
       <c r="A158" s="5" t="s">
-        <v>194</v>
+        <v>152</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>1629</v>
+        <v>1619</v>
       </c>
       <c r="C158" s="3">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>195</v>
+        <v>153</v>
       </c>
       <c r="E158" s="4" t="s">
-        <v>196</v>
+        <v>154</v>
+      </c>
+      <c r="F158" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="G158" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H158" s="5" t="s">
+        <v>2085</v>
+      </c>
+      <c r="I158" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="J158" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="K158" s="5" t="s">
+        <v>2088</v>
+      </c>
+      <c r="L158" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="M158" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="N158" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="O158" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="P158" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="Q158" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="R158" s="5" t="s">
+        <v>1349</v>
+      </c>
+      <c r="S158" s="5" t="s">
+        <v>2086</v>
+      </c>
+      <c r="T158" s="5" t="s">
+        <v>1972</v>
+      </c>
+      <c r="U158" s="5" t="s">
+        <v>1353</v>
+      </c>
+      <c r="V158" s="5" t="s">
+        <v>2089</v>
+      </c>
+      <c r="W158" s="5" t="s">
+        <v>2092</v>
+      </c>
+      <c r="X158" s="5" t="s">
+        <v>2093</v>
+      </c>
+      <c r="Y158" s="5" t="s">
+        <v>2087</v>
+      </c>
+      <c r="Z158" s="5" t="s">
+        <v>2094</v>
+      </c>
+      <c r="AA158" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="AB158" s="5" t="s">
+        <v>2091</v>
+      </c>
+      <c r="AC158" s="5" t="s">
+        <v>2090</v>
+      </c>
+      <c r="AD158" s="5" t="s">
+        <v>1342</v>
       </c>
       <c r="AE158" s="5" t="b">
         <f>NOT(OR(ISBLANK(Table4[[#This Row],[DE1: name]]),ISBLANK(Table4[[#This Row],[DE2: extended version]]),ISBLANK(Table4[[#This Row],[DE3: long-term]]),ISBLANK(Table4[[#This Row],[DE4: local+map]]),ISBLANK(Table4[[#This Row],[DE5: localizer]]),ISBLANK(Table4[[#This Row],[DE6: map]]),ISBLANK(Table4[[#This Row],[DE7: active SLAM]]),ISBLANK(Table4[[#This Row],[DE8: SPLAM]]),ISBLANK(Table4[[#This Row],[DE9: VT&amp;R]]),ISBLANK(Table4[[#This Row],[DE10: multi-robot]]),ISBLANK(Table4[[#This Row],[DE11: prior]]),ISBLANK(Table4[[#This Row],[DE12: learning]]),ISBLANK(Table4[[#This Row],[DE13: computation]]),ISBLANK(Table4[[#This Row],[DE14: online/offline]]),ISBLANK(Table4[[#This Row],[DE15: environ]]),ISBLANK(Table4[[#This Row],[DE16: domain]]),ISBLANK(Table4[[#This Row],[DE17: sensor]]),ISBLANK(Table4[[#This Row],[DE18: error eval]]),ISBLANK(Table4[[#This Row],[DE19: compute eval]]),ISBLANK(Table4[[#This Row],[DE20: gt data]]),ISBLANK(Table4[[#This Row],[DE21: repo link]]),ISBLANK(Table4[[#This Row],[DE22: datasets]]),ISBLANK(Table4[[#This Row],[DE23: distance]]),ISBLANK(Table4[[#This Row],[DE24: time]])))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF158" s="5" t="b">
         <f>AND(Table4[[#This Row],[all data?]],NOT(OR(Table4[[#This Row],[DE1: name]]="?",Table4[[#This Row],[DE2: extended version]]="?",Table4[[#This Row],[DE3: long-term]]="?",Table4[[#This Row],[DE4: local+map]]="?",Table4[[#This Row],[DE5: localizer]]="?",Table4[[#This Row],[DE6: map]]="?",Table4[[#This Row],[DE7: active SLAM]]="?",Table4[[#This Row],[DE8: SPLAM]]="?",Table4[[#This Row],[DE9: VT&amp;R]]="?",Table4[[#This Row],[DE10: multi-robot]]="?",Table4[[#This Row],[DE11: prior]]="?",Table4[[#This Row],[DE12: learning]]="?",Table4[[#This Row],[DE13: computation]]="?",Table4[[#This Row],[DE14: online/offline]]="?",Table4[[#This Row],[DE15: environ]]="?",Table4[[#This Row],[DE16: domain]]="?",Table4[[#This Row],[DE17: sensor]]="?",Table4[[#This Row],[DE18: error eval]]="?",Table4[[#This Row],[DE19: compute eval]]="?",Table4[[#This Row],[DE20: gt data]]="?",Table4[[#This Row],[DE21: repo link]]="?",Table4[[#This Row],[DE22: datasets]]="?",Table4[[#This Row],[DE23: distance]]="?",Table4[[#This Row],[DE24: time]]="?")))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG158" s="5" t="s">
         <v>1434</v>
@@ -51487,25 +51621,28 @@
     </row>
     <row r="159" spans="1:33" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A159" s="5" t="s">
-        <v>230</v>
+        <v>158</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>1639</v>
+        <v>1607</v>
       </c>
       <c r="C159" s="3">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>231</v>
+        <v>159</v>
       </c>
       <c r="E159" s="4" t="s">
-        <v>232</v>
+        <v>160</v>
       </c>
       <c r="F159" s="5" t="s">
-        <v>2299</v>
+        <v>1968</v>
       </c>
       <c r="G159" s="5" t="s">
         <v>1342</v>
+      </c>
+      <c r="AD159" s="5" t="s">
+        <v>2110</v>
       </c>
       <c r="AE159" s="5" t="b">
         <f>NOT(OR(ISBLANK(Table4[[#This Row],[DE1: name]]),ISBLANK(Table4[[#This Row],[DE2: extended version]]),ISBLANK(Table4[[#This Row],[DE3: long-term]]),ISBLANK(Table4[[#This Row],[DE4: local+map]]),ISBLANK(Table4[[#This Row],[DE5: localizer]]),ISBLANK(Table4[[#This Row],[DE6: map]]),ISBLANK(Table4[[#This Row],[DE7: active SLAM]]),ISBLANK(Table4[[#This Row],[DE8: SPLAM]]),ISBLANK(Table4[[#This Row],[DE9: VT&amp;R]]),ISBLANK(Table4[[#This Row],[DE10: multi-robot]]),ISBLANK(Table4[[#This Row],[DE11: prior]]),ISBLANK(Table4[[#This Row],[DE12: learning]]),ISBLANK(Table4[[#This Row],[DE13: computation]]),ISBLANK(Table4[[#This Row],[DE14: online/offline]]),ISBLANK(Table4[[#This Row],[DE15: environ]]),ISBLANK(Table4[[#This Row],[DE16: domain]]),ISBLANK(Table4[[#This Row],[DE17: sensor]]),ISBLANK(Table4[[#This Row],[DE18: error eval]]),ISBLANK(Table4[[#This Row],[DE19: compute eval]]),ISBLANK(Table4[[#This Row],[DE20: gt data]]),ISBLANK(Table4[[#This Row],[DE21: repo link]]),ISBLANK(Table4[[#This Row],[DE22: datasets]]),ISBLANK(Table4[[#This Row],[DE23: distance]]),ISBLANK(Table4[[#This Row],[DE24: time]])))</f>
@@ -51519,124 +51656,67 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="160" spans="1:33" ht="132" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:33" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A160" s="5" t="s">
-        <v>236</v>
+        <v>161</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>1641</v>
+        <v>1607</v>
       </c>
       <c r="C160" s="3">
-        <v>2016</v>
+        <v>2013</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>237</v>
+        <v>162</v>
       </c>
       <c r="E160" s="4" t="s">
-        <v>238</v>
+        <v>163</v>
       </c>
       <c r="F160" s="5" t="s">
-        <v>1342</v>
+        <v>1968</v>
       </c>
       <c r="G160" s="5" t="s">
         <v>1342</v>
       </c>
-      <c r="H160" s="5" t="s">
-        <v>2337</v>
-      </c>
-      <c r="I160" s="5" t="s">
-        <v>2045</v>
-      </c>
-      <c r="J160" s="5" t="s">
-        <v>2335</v>
-      </c>
-      <c r="K160" s="5" t="s">
-        <v>2336</v>
-      </c>
-      <c r="L160" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="M160" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="N160" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="O160" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="P160" s="5" t="s">
-        <v>2329</v>
-      </c>
-      <c r="Q160" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="R160" s="5" t="s">
-        <v>1349</v>
-      </c>
-      <c r="S160" s="5" t="s">
-        <v>2330</v>
-      </c>
-      <c r="T160" s="5" t="s">
-        <v>1399</v>
-      </c>
-      <c r="U160" s="5" t="s">
-        <v>2331</v>
-      </c>
-      <c r="V160" s="5" t="s">
-        <v>2334</v>
-      </c>
-      <c r="W160" s="5" t="s">
-        <v>2340</v>
-      </c>
-      <c r="X160" s="5" t="s">
-        <v>1342</v>
-      </c>
-      <c r="Y160" s="5" t="s">
-        <v>2338</v>
-      </c>
-      <c r="Z160" s="5" t="s">
-        <v>1342</v>
-      </c>
-      <c r="AA160" s="5" t="s">
-        <v>1342</v>
-      </c>
-      <c r="AB160" s="5" t="s">
-        <v>1342</v>
-      </c>
-      <c r="AC160" s="5" t="s">
-        <v>2339</v>
-      </c>
       <c r="AD160" s="5" t="s">
-        <v>2328</v>
+        <v>2110</v>
       </c>
       <c r="AE160" s="5" t="b">
         <f>NOT(OR(ISBLANK(Table4[[#This Row],[DE1: name]]),ISBLANK(Table4[[#This Row],[DE2: extended version]]),ISBLANK(Table4[[#This Row],[DE3: long-term]]),ISBLANK(Table4[[#This Row],[DE4: local+map]]),ISBLANK(Table4[[#This Row],[DE5: localizer]]),ISBLANK(Table4[[#This Row],[DE6: map]]),ISBLANK(Table4[[#This Row],[DE7: active SLAM]]),ISBLANK(Table4[[#This Row],[DE8: SPLAM]]),ISBLANK(Table4[[#This Row],[DE9: VT&amp;R]]),ISBLANK(Table4[[#This Row],[DE10: multi-robot]]),ISBLANK(Table4[[#This Row],[DE11: prior]]),ISBLANK(Table4[[#This Row],[DE12: learning]]),ISBLANK(Table4[[#This Row],[DE13: computation]]),ISBLANK(Table4[[#This Row],[DE14: online/offline]]),ISBLANK(Table4[[#This Row],[DE15: environ]]),ISBLANK(Table4[[#This Row],[DE16: domain]]),ISBLANK(Table4[[#This Row],[DE17: sensor]]),ISBLANK(Table4[[#This Row],[DE18: error eval]]),ISBLANK(Table4[[#This Row],[DE19: compute eval]]),ISBLANK(Table4[[#This Row],[DE20: gt data]]),ISBLANK(Table4[[#This Row],[DE21: repo link]]),ISBLANK(Table4[[#This Row],[DE22: datasets]]),ISBLANK(Table4[[#This Row],[DE23: distance]]),ISBLANK(Table4[[#This Row],[DE24: time]])))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF160" s="5" t="b">
         <f>AND(Table4[[#This Row],[all data?]],NOT(OR(Table4[[#This Row],[DE1: name]]="?",Table4[[#This Row],[DE2: extended version]]="?",Table4[[#This Row],[DE3: long-term]]="?",Table4[[#This Row],[DE4: local+map]]="?",Table4[[#This Row],[DE5: localizer]]="?",Table4[[#This Row],[DE6: map]]="?",Table4[[#This Row],[DE7: active SLAM]]="?",Table4[[#This Row],[DE8: SPLAM]]="?",Table4[[#This Row],[DE9: VT&amp;R]]="?",Table4[[#This Row],[DE10: multi-robot]]="?",Table4[[#This Row],[DE11: prior]]="?",Table4[[#This Row],[DE12: learning]]="?",Table4[[#This Row],[DE13: computation]]="?",Table4[[#This Row],[DE14: online/offline]]="?",Table4[[#This Row],[DE15: environ]]="?",Table4[[#This Row],[DE16: domain]]="?",Table4[[#This Row],[DE17: sensor]]="?",Table4[[#This Row],[DE18: error eval]]="?",Table4[[#This Row],[DE19: compute eval]]="?",Table4[[#This Row],[DE20: gt data]]="?",Table4[[#This Row],[DE21: repo link]]="?",Table4[[#This Row],[DE22: datasets]]="?",Table4[[#This Row],[DE23: distance]]="?",Table4[[#This Row],[DE24: time]]="?")))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG160" s="5" t="s">
         <v>1434</v>
       </c>
     </row>
-    <row r="161" spans="1:33" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:33" ht="66" x14ac:dyDescent="0.3">
       <c r="A161" s="5" t="s">
-        <v>242</v>
+        <v>179</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>1643</v>
+        <v>1624</v>
       </c>
       <c r="C161" s="3">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>243</v>
+        <v>180</v>
       </c>
       <c r="E161" s="4" t="s">
-        <v>244</v>
+        <v>181</v>
+      </c>
+      <c r="F161" s="5" t="s">
+        <v>2149</v>
+      </c>
+      <c r="G161" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="AD161" s="5" t="s">
+        <v>2150</v>
       </c>
       <c r="AE161" s="5" t="b">
         <f>NOT(OR(ISBLANK(Table4[[#This Row],[DE1: name]]),ISBLANK(Table4[[#This Row],[DE2: extended version]]),ISBLANK(Table4[[#This Row],[DE3: long-term]]),ISBLANK(Table4[[#This Row],[DE4: local+map]]),ISBLANK(Table4[[#This Row],[DE5: localizer]]),ISBLANK(Table4[[#This Row],[DE6: map]]),ISBLANK(Table4[[#This Row],[DE7: active SLAM]]),ISBLANK(Table4[[#This Row],[DE8: SPLAM]]),ISBLANK(Table4[[#This Row],[DE9: VT&amp;R]]),ISBLANK(Table4[[#This Row],[DE10: multi-robot]]),ISBLANK(Table4[[#This Row],[DE11: prior]]),ISBLANK(Table4[[#This Row],[DE12: learning]]),ISBLANK(Table4[[#This Row],[DE13: computation]]),ISBLANK(Table4[[#This Row],[DE14: online/offline]]),ISBLANK(Table4[[#This Row],[DE15: environ]]),ISBLANK(Table4[[#This Row],[DE16: domain]]),ISBLANK(Table4[[#This Row],[DE17: sensor]]),ISBLANK(Table4[[#This Row],[DE18: error eval]]),ISBLANK(Table4[[#This Row],[DE19: compute eval]]),ISBLANK(Table4[[#This Row],[DE20: gt data]]),ISBLANK(Table4[[#This Row],[DE21: repo link]]),ISBLANK(Table4[[#This Row],[DE22: datasets]]),ISBLANK(Table4[[#This Row],[DE23: distance]]),ISBLANK(Table4[[#This Row],[DE24: time]])))</f>
@@ -51650,133 +51730,55 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="162" spans="1:33" ht="145.19999999999999" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:33" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A162" s="5" t="s">
-        <v>245</v>
+        <v>194</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>1644</v>
+        <v>1629</v>
       </c>
       <c r="C162" s="3">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>246</v>
+        <v>195</v>
       </c>
       <c r="E162" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="F162" s="5" t="s">
-        <v>1342</v>
-      </c>
-      <c r="G162" s="5" t="s">
-        <v>1342</v>
-      </c>
-      <c r="H162" s="5" t="s">
-        <v>2376</v>
-      </c>
-      <c r="I162" s="5" t="s">
-        <v>2374</v>
-      </c>
-      <c r="J162" s="5" t="s">
-        <v>2375</v>
-      </c>
-      <c r="K162" s="5" t="s">
-        <v>2373</v>
-      </c>
-      <c r="L162" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="M162" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="N162" s="5" t="s">
-        <v>2369</v>
-      </c>
-      <c r="O162" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="P162" s="5" t="s">
-        <v>2371</v>
-      </c>
-      <c r="Q162" s="5" t="s">
-        <v>2370</v>
-      </c>
-      <c r="R162" s="5" t="s">
-        <v>1349</v>
-      </c>
-      <c r="S162" s="5" t="s">
-        <v>2097</v>
-      </c>
-      <c r="T162" s="5" t="s">
-        <v>1399</v>
-      </c>
-      <c r="U162" s="5" t="s">
-        <v>1353</v>
-      </c>
-      <c r="V162" s="5" t="s">
-        <v>2372</v>
-      </c>
-      <c r="W162" s="5" t="s">
-        <v>2377</v>
-      </c>
-      <c r="X162" s="5" t="s">
-        <v>2378</v>
-      </c>
-      <c r="Y162" s="5" t="s">
-        <v>1342</v>
-      </c>
-      <c r="Z162" s="5" t="s">
-        <v>1342</v>
-      </c>
-      <c r="AA162" s="5" t="s">
-        <v>1342</v>
-      </c>
-      <c r="AB162" s="5" t="s">
-        <v>2379</v>
-      </c>
-      <c r="AC162" s="5" t="s">
-        <v>2380</v>
-      </c>
-      <c r="AD162" s="5" t="s">
-        <v>1342</v>
+        <v>196</v>
       </c>
       <c r="AE162" s="5" t="b">
         <f>NOT(OR(ISBLANK(Table4[[#This Row],[DE1: name]]),ISBLANK(Table4[[#This Row],[DE2: extended version]]),ISBLANK(Table4[[#This Row],[DE3: long-term]]),ISBLANK(Table4[[#This Row],[DE4: local+map]]),ISBLANK(Table4[[#This Row],[DE5: localizer]]),ISBLANK(Table4[[#This Row],[DE6: map]]),ISBLANK(Table4[[#This Row],[DE7: active SLAM]]),ISBLANK(Table4[[#This Row],[DE8: SPLAM]]),ISBLANK(Table4[[#This Row],[DE9: VT&amp;R]]),ISBLANK(Table4[[#This Row],[DE10: multi-robot]]),ISBLANK(Table4[[#This Row],[DE11: prior]]),ISBLANK(Table4[[#This Row],[DE12: learning]]),ISBLANK(Table4[[#This Row],[DE13: computation]]),ISBLANK(Table4[[#This Row],[DE14: online/offline]]),ISBLANK(Table4[[#This Row],[DE15: environ]]),ISBLANK(Table4[[#This Row],[DE16: domain]]),ISBLANK(Table4[[#This Row],[DE17: sensor]]),ISBLANK(Table4[[#This Row],[DE18: error eval]]),ISBLANK(Table4[[#This Row],[DE19: compute eval]]),ISBLANK(Table4[[#This Row],[DE20: gt data]]),ISBLANK(Table4[[#This Row],[DE21: repo link]]),ISBLANK(Table4[[#This Row],[DE22: datasets]]),ISBLANK(Table4[[#This Row],[DE23: distance]]),ISBLANK(Table4[[#This Row],[DE24: time]])))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF162" s="5" t="b">
         <f>AND(Table4[[#This Row],[all data?]],NOT(OR(Table4[[#This Row],[DE1: name]]="?",Table4[[#This Row],[DE2: extended version]]="?",Table4[[#This Row],[DE3: long-term]]="?",Table4[[#This Row],[DE4: local+map]]="?",Table4[[#This Row],[DE5: localizer]]="?",Table4[[#This Row],[DE6: map]]="?",Table4[[#This Row],[DE7: active SLAM]]="?",Table4[[#This Row],[DE8: SPLAM]]="?",Table4[[#This Row],[DE9: VT&amp;R]]="?",Table4[[#This Row],[DE10: multi-robot]]="?",Table4[[#This Row],[DE11: prior]]="?",Table4[[#This Row],[DE12: learning]]="?",Table4[[#This Row],[DE13: computation]]="?",Table4[[#This Row],[DE14: online/offline]]="?",Table4[[#This Row],[DE15: environ]]="?",Table4[[#This Row],[DE16: domain]]="?",Table4[[#This Row],[DE17: sensor]]="?",Table4[[#This Row],[DE18: error eval]]="?",Table4[[#This Row],[DE19: compute eval]]="?",Table4[[#This Row],[DE20: gt data]]="?",Table4[[#This Row],[DE21: repo link]]="?",Table4[[#This Row],[DE22: datasets]]="?",Table4[[#This Row],[DE23: distance]]="?",Table4[[#This Row],[DE24: time]]="?")))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG162" s="5" t="s">
         <v>1434</v>
       </c>
     </row>
-    <row r="163" spans="1:33" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:33" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A163" s="5" t="s">
-        <v>272</v>
+        <v>230</v>
       </c>
       <c r="B163" s="3" t="s">
         <v>1639</v>
       </c>
       <c r="C163" s="3">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>273</v>
+        <v>231</v>
       </c>
       <c r="E163" s="4" t="s">
-        <v>274</v>
+        <v>232</v>
       </c>
       <c r="F163" s="5" t="s">
-        <v>2300</v>
+        <v>2299</v>
       </c>
       <c r="G163" s="5" t="s">
         <v>1342</v>
-      </c>
-      <c r="Z163" s="5" t="s">
-        <v>2301</v>
       </c>
       <c r="AE163" s="5" t="b">
         <f>NOT(OR(ISBLANK(Table4[[#This Row],[DE1: name]]),ISBLANK(Table4[[#This Row],[DE2: extended version]]),ISBLANK(Table4[[#This Row],[DE3: long-term]]),ISBLANK(Table4[[#This Row],[DE4: local+map]]),ISBLANK(Table4[[#This Row],[DE5: localizer]]),ISBLANK(Table4[[#This Row],[DE6: map]]),ISBLANK(Table4[[#This Row],[DE7: active SLAM]]),ISBLANK(Table4[[#This Row],[DE8: SPLAM]]),ISBLANK(Table4[[#This Row],[DE9: VT&amp;R]]),ISBLANK(Table4[[#This Row],[DE10: multi-robot]]),ISBLANK(Table4[[#This Row],[DE11: prior]]),ISBLANK(Table4[[#This Row],[DE12: learning]]),ISBLANK(Table4[[#This Row],[DE13: computation]]),ISBLANK(Table4[[#This Row],[DE14: online/offline]]),ISBLANK(Table4[[#This Row],[DE15: environ]]),ISBLANK(Table4[[#This Row],[DE16: domain]]),ISBLANK(Table4[[#This Row],[DE17: sensor]]),ISBLANK(Table4[[#This Row],[DE18: error eval]]),ISBLANK(Table4[[#This Row],[DE19: compute eval]]),ISBLANK(Table4[[#This Row],[DE20: gt data]]),ISBLANK(Table4[[#This Row],[DE21: repo link]]),ISBLANK(Table4[[#This Row],[DE22: datasets]]),ISBLANK(Table4[[#This Row],[DE23: distance]]),ISBLANK(Table4[[#This Row],[DE24: time]])))</f>
@@ -51790,173 +51792,170 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="164" spans="1:33" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:33" ht="132" x14ac:dyDescent="0.3">
       <c r="A164" s="5" t="s">
-        <v>275</v>
+        <v>236</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>1653</v>
+        <v>1641</v>
       </c>
       <c r="C164" s="3">
         <v>2016</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>276</v>
+        <v>237</v>
       </c>
       <c r="E164" s="4" t="s">
-        <v>277</v>
+        <v>238</v>
       </c>
       <c r="F164" s="5" t="s">
-        <v>2402</v>
+        <v>1342</v>
       </c>
       <c r="G164" s="5" t="s">
         <v>1342</v>
+      </c>
+      <c r="H164" s="5" t="s">
+        <v>2337</v>
+      </c>
+      <c r="I164" s="5" t="s">
+        <v>2045</v>
+      </c>
+      <c r="J164" s="5" t="s">
+        <v>2335</v>
+      </c>
+      <c r="K164" s="5" t="s">
+        <v>2336</v>
+      </c>
+      <c r="L164" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="M164" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="N164" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="O164" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="P164" s="5" t="s">
+        <v>2329</v>
+      </c>
+      <c r="Q164" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="R164" s="5" t="s">
+        <v>1349</v>
+      </c>
+      <c r="S164" s="5" t="s">
+        <v>2330</v>
+      </c>
+      <c r="T164" s="5" t="s">
+        <v>1399</v>
+      </c>
+      <c r="U164" s="5" t="s">
+        <v>2331</v>
+      </c>
+      <c r="V164" s="5" t="s">
+        <v>2334</v>
+      </c>
+      <c r="W164" s="5" t="s">
+        <v>2340</v>
+      </c>
+      <c r="X164" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="Y164" s="5" t="s">
+        <v>2338</v>
+      </c>
+      <c r="Z164" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="AA164" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="AB164" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="AC164" s="5" t="s">
+        <v>2339</v>
+      </c>
+      <c r="AD164" s="5" t="s">
+        <v>2328</v>
       </c>
       <c r="AE164" s="5" t="b">
         <f>NOT(OR(ISBLANK(Table4[[#This Row],[DE1: name]]),ISBLANK(Table4[[#This Row],[DE2: extended version]]),ISBLANK(Table4[[#This Row],[DE3: long-term]]),ISBLANK(Table4[[#This Row],[DE4: local+map]]),ISBLANK(Table4[[#This Row],[DE5: localizer]]),ISBLANK(Table4[[#This Row],[DE6: map]]),ISBLANK(Table4[[#This Row],[DE7: active SLAM]]),ISBLANK(Table4[[#This Row],[DE8: SPLAM]]),ISBLANK(Table4[[#This Row],[DE9: VT&amp;R]]),ISBLANK(Table4[[#This Row],[DE10: multi-robot]]),ISBLANK(Table4[[#This Row],[DE11: prior]]),ISBLANK(Table4[[#This Row],[DE12: learning]]),ISBLANK(Table4[[#This Row],[DE13: computation]]),ISBLANK(Table4[[#This Row],[DE14: online/offline]]),ISBLANK(Table4[[#This Row],[DE15: environ]]),ISBLANK(Table4[[#This Row],[DE16: domain]]),ISBLANK(Table4[[#This Row],[DE17: sensor]]),ISBLANK(Table4[[#This Row],[DE18: error eval]]),ISBLANK(Table4[[#This Row],[DE19: compute eval]]),ISBLANK(Table4[[#This Row],[DE20: gt data]]),ISBLANK(Table4[[#This Row],[DE21: repo link]]),ISBLANK(Table4[[#This Row],[DE22: datasets]]),ISBLANK(Table4[[#This Row],[DE23: distance]]),ISBLANK(Table4[[#This Row],[DE24: time]])))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF164" s="5" t="b">
         <f>AND(Table4[[#This Row],[all data?]],NOT(OR(Table4[[#This Row],[DE1: name]]="?",Table4[[#This Row],[DE2: extended version]]="?",Table4[[#This Row],[DE3: long-term]]="?",Table4[[#This Row],[DE4: local+map]]="?",Table4[[#This Row],[DE5: localizer]]="?",Table4[[#This Row],[DE6: map]]="?",Table4[[#This Row],[DE7: active SLAM]]="?",Table4[[#This Row],[DE8: SPLAM]]="?",Table4[[#This Row],[DE9: VT&amp;R]]="?",Table4[[#This Row],[DE10: multi-robot]]="?",Table4[[#This Row],[DE11: prior]]="?",Table4[[#This Row],[DE12: learning]]="?",Table4[[#This Row],[DE13: computation]]="?",Table4[[#This Row],[DE14: online/offline]]="?",Table4[[#This Row],[DE15: environ]]="?",Table4[[#This Row],[DE16: domain]]="?",Table4[[#This Row],[DE17: sensor]]="?",Table4[[#This Row],[DE18: error eval]]="?",Table4[[#This Row],[DE19: compute eval]]="?",Table4[[#This Row],[DE20: gt data]]="?",Table4[[#This Row],[DE21: repo link]]="?",Table4[[#This Row],[DE22: datasets]]="?",Table4[[#This Row],[DE23: distance]]="?",Table4[[#This Row],[DE24: time]]="?")))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG164" s="5" t="s">
         <v>1434</v>
       </c>
     </row>
-    <row r="165" spans="1:33" ht="145.19999999999999" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:33" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A165" s="5" t="s">
-        <v>278</v>
+        <v>242</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>1654</v>
+        <v>1643</v>
       </c>
       <c r="C165" s="3">
         <v>2016</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>279</v>
+        <v>243</v>
       </c>
       <c r="E165" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="F165" s="5" t="s">
-        <v>2437</v>
-      </c>
-      <c r="G165" s="5" t="s">
-        <v>1342</v>
-      </c>
-      <c r="H165" s="5" t="s">
-        <v>2438</v>
-      </c>
-      <c r="I165" s="5" t="s">
-        <v>1342</v>
-      </c>
-      <c r="J165" s="5" t="s">
-        <v>2440</v>
-      </c>
-      <c r="K165" s="5" t="s">
-        <v>1342</v>
-      </c>
-      <c r="L165" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="M165" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="N165" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="O165" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="P165" s="5" t="s">
-        <v>2439</v>
-      </c>
-      <c r="Q165" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="R165" s="5" t="s">
-        <v>1342</v>
-      </c>
-      <c r="S165" s="5" t="s">
-        <v>1342</v>
-      </c>
-      <c r="T165" s="5" t="s">
-        <v>1399</v>
-      </c>
-      <c r="U165" s="5" t="s">
-        <v>1353</v>
-      </c>
-      <c r="V165" s="5" t="s">
-        <v>1357</v>
-      </c>
-      <c r="W165" s="5" t="s">
-        <v>2441</v>
-      </c>
-      <c r="X165" s="5" t="s">
-        <v>1342</v>
-      </c>
-      <c r="Y165" s="5" t="s">
-        <v>2442</v>
-      </c>
-      <c r="Z165" s="5" t="s">
-        <v>1342</v>
-      </c>
-      <c r="AA165" s="5" t="s">
-        <v>2445</v>
-      </c>
-      <c r="AB165" s="5" t="s">
-        <v>2443</v>
-      </c>
-      <c r="AC165" s="5" t="s">
-        <v>2444</v>
-      </c>
-      <c r="AD165" s="5" t="s">
-        <v>2446</v>
+        <v>244</v>
       </c>
       <c r="AE165" s="5" t="b">
         <f>NOT(OR(ISBLANK(Table4[[#This Row],[DE1: name]]),ISBLANK(Table4[[#This Row],[DE2: extended version]]),ISBLANK(Table4[[#This Row],[DE3: long-term]]),ISBLANK(Table4[[#This Row],[DE4: local+map]]),ISBLANK(Table4[[#This Row],[DE5: localizer]]),ISBLANK(Table4[[#This Row],[DE6: map]]),ISBLANK(Table4[[#This Row],[DE7: active SLAM]]),ISBLANK(Table4[[#This Row],[DE8: SPLAM]]),ISBLANK(Table4[[#This Row],[DE9: VT&amp;R]]),ISBLANK(Table4[[#This Row],[DE10: multi-robot]]),ISBLANK(Table4[[#This Row],[DE11: prior]]),ISBLANK(Table4[[#This Row],[DE12: learning]]),ISBLANK(Table4[[#This Row],[DE13: computation]]),ISBLANK(Table4[[#This Row],[DE14: online/offline]]),ISBLANK(Table4[[#This Row],[DE15: environ]]),ISBLANK(Table4[[#This Row],[DE16: domain]]),ISBLANK(Table4[[#This Row],[DE17: sensor]]),ISBLANK(Table4[[#This Row],[DE18: error eval]]),ISBLANK(Table4[[#This Row],[DE19: compute eval]]),ISBLANK(Table4[[#This Row],[DE20: gt data]]),ISBLANK(Table4[[#This Row],[DE21: repo link]]),ISBLANK(Table4[[#This Row],[DE22: datasets]]),ISBLANK(Table4[[#This Row],[DE23: distance]]),ISBLANK(Table4[[#This Row],[DE24: time]])))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF165" s="5" t="b">
         <f>AND(Table4[[#This Row],[all data?]],NOT(OR(Table4[[#This Row],[DE1: name]]="?",Table4[[#This Row],[DE2: extended version]]="?",Table4[[#This Row],[DE3: long-term]]="?",Table4[[#This Row],[DE4: local+map]]="?",Table4[[#This Row],[DE5: localizer]]="?",Table4[[#This Row],[DE6: map]]="?",Table4[[#This Row],[DE7: active SLAM]]="?",Table4[[#This Row],[DE8: SPLAM]]="?",Table4[[#This Row],[DE9: VT&amp;R]]="?",Table4[[#This Row],[DE10: multi-robot]]="?",Table4[[#This Row],[DE11: prior]]="?",Table4[[#This Row],[DE12: learning]]="?",Table4[[#This Row],[DE13: computation]]="?",Table4[[#This Row],[DE14: online/offline]]="?",Table4[[#This Row],[DE15: environ]]="?",Table4[[#This Row],[DE16: domain]]="?",Table4[[#This Row],[DE17: sensor]]="?",Table4[[#This Row],[DE18: error eval]]="?",Table4[[#This Row],[DE19: compute eval]]="?",Table4[[#This Row],[DE20: gt data]]="?",Table4[[#This Row],[DE21: repo link]]="?",Table4[[#This Row],[DE22: datasets]]="?",Table4[[#This Row],[DE23: distance]]="?",Table4[[#This Row],[DE24: time]]="?")))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG165" s="5" t="s">
         <v>1434</v>
       </c>
     </row>
-    <row r="166" spans="1:33" ht="132" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:33" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A166" s="5" t="s">
-        <v>335</v>
+        <v>245</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>1670</v>
+        <v>1644</v>
       </c>
       <c r="C166" s="3">
-        <v>2018</v>
+        <v>2016</v>
+      </c>
+      <c r="D166" s="3" t="s">
+        <v>246</v>
       </c>
       <c r="E166" s="4" t="s">
-        <v>336</v>
+        <v>247</v>
       </c>
       <c r="F166" s="5" t="s">
-        <v>2531</v>
+        <v>1342</v>
       </c>
       <c r="G166" s="5" t="s">
         <v>1342</v>
       </c>
       <c r="H166" s="5" t="s">
-        <v>2549</v>
+        <v>2376</v>
       </c>
       <c r="I166" s="5" t="s">
-        <v>1342</v>
+        <v>2374</v>
       </c>
       <c r="J166" s="5" t="s">
-        <v>2551</v>
+        <v>2375</v>
       </c>
       <c r="K166" s="5" t="s">
-        <v>1342</v>
+        <v>2373</v>
       </c>
       <c r="L166" s="5" t="s">
         <v>655</v>
@@ -51965,22 +51964,22 @@
         <v>655</v>
       </c>
       <c r="N166" s="5" t="s">
-        <v>655</v>
+        <v>2369</v>
       </c>
       <c r="O166" s="5" t="s">
         <v>655</v>
       </c>
       <c r="P166" s="5" t="s">
-        <v>655</v>
+        <v>2371</v>
       </c>
       <c r="Q166" s="5" t="s">
-        <v>2550</v>
+        <v>2370</v>
       </c>
       <c r="R166" s="5" t="s">
-        <v>1342</v>
+        <v>1349</v>
       </c>
       <c r="S166" s="5" t="s">
-        <v>1342</v>
+        <v>2097</v>
       </c>
       <c r="T166" s="5" t="s">
         <v>1399</v>
@@ -51989,28 +51988,28 @@
         <v>1353</v>
       </c>
       <c r="V166" s="5" t="s">
-        <v>1357</v>
+        <v>2372</v>
       </c>
       <c r="W166" s="5" t="s">
-        <v>1536</v>
+        <v>2377</v>
       </c>
       <c r="X166" s="5" t="s">
-        <v>1342</v>
+        <v>2378</v>
       </c>
       <c r="Y166" s="5" t="s">
-        <v>2538</v>
+        <v>1342</v>
       </c>
       <c r="Z166" s="5" t="s">
         <v>1342</v>
       </c>
       <c r="AA166" s="5" t="s">
-        <v>2534</v>
+        <v>1342</v>
       </c>
       <c r="AB166" s="5" t="s">
-        <v>2536</v>
+        <v>2379</v>
       </c>
       <c r="AC166" s="5" t="s">
-        <v>2537</v>
+        <v>2380</v>
       </c>
       <c r="AD166" s="5" t="s">
         <v>1342</v>
@@ -52027,21 +52026,30 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="167" spans="1:33" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:33" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A167" s="5" t="s">
-        <v>349</v>
+        <v>272</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>1674</v>
+        <v>1639</v>
       </c>
       <c r="C167" s="3">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>350</v>
+        <v>273</v>
       </c>
       <c r="E167" s="4" t="s">
-        <v>351</v>
+        <v>274</v>
+      </c>
+      <c r="F167" s="5" t="s">
+        <v>2300</v>
+      </c>
+      <c r="G167" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="Z167" s="5" t="s">
+        <v>2301</v>
       </c>
       <c r="AE167" s="5" t="b">
         <f>NOT(OR(ISBLANK(Table4[[#This Row],[DE1: name]]),ISBLANK(Table4[[#This Row],[DE2: extended version]]),ISBLANK(Table4[[#This Row],[DE3: long-term]]),ISBLANK(Table4[[#This Row],[DE4: local+map]]),ISBLANK(Table4[[#This Row],[DE5: localizer]]),ISBLANK(Table4[[#This Row],[DE6: map]]),ISBLANK(Table4[[#This Row],[DE7: active SLAM]]),ISBLANK(Table4[[#This Row],[DE8: SPLAM]]),ISBLANK(Table4[[#This Row],[DE9: VT&amp;R]]),ISBLANK(Table4[[#This Row],[DE10: multi-robot]]),ISBLANK(Table4[[#This Row],[DE11: prior]]),ISBLANK(Table4[[#This Row],[DE12: learning]]),ISBLANK(Table4[[#This Row],[DE13: computation]]),ISBLANK(Table4[[#This Row],[DE14: online/offline]]),ISBLANK(Table4[[#This Row],[DE15: environ]]),ISBLANK(Table4[[#This Row],[DE16: domain]]),ISBLANK(Table4[[#This Row],[DE17: sensor]]),ISBLANK(Table4[[#This Row],[DE18: error eval]]),ISBLANK(Table4[[#This Row],[DE19: compute eval]]),ISBLANK(Table4[[#This Row],[DE20: gt data]]),ISBLANK(Table4[[#This Row],[DE21: repo link]]),ISBLANK(Table4[[#This Row],[DE22: datasets]]),ISBLANK(Table4[[#This Row],[DE23: distance]]),ISBLANK(Table4[[#This Row],[DE24: time]])))</f>
@@ -52057,19 +52065,25 @@
     </row>
     <row r="168" spans="1:33" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A168" s="5" t="s">
-        <v>424</v>
+        <v>275</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>1699</v>
+        <v>1653</v>
       </c>
       <c r="C168" s="3">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>425</v>
+        <v>276</v>
       </c>
       <c r="E168" s="4" t="s">
-        <v>426</v>
+        <v>277</v>
+      </c>
+      <c r="F168" s="5" t="s">
+        <v>2402</v>
+      </c>
+      <c r="G168" s="5" t="s">
+        <v>1342</v>
       </c>
       <c r="AE168" s="5" t="b">
         <f>NOT(OR(ISBLANK(Table4[[#This Row],[DE1: name]]),ISBLANK(Table4[[#This Row],[DE2: extended version]]),ISBLANK(Table4[[#This Row],[DE3: long-term]]),ISBLANK(Table4[[#This Row],[DE4: local+map]]),ISBLANK(Table4[[#This Row],[DE5: localizer]]),ISBLANK(Table4[[#This Row],[DE6: map]]),ISBLANK(Table4[[#This Row],[DE7: active SLAM]]),ISBLANK(Table4[[#This Row],[DE8: SPLAM]]),ISBLANK(Table4[[#This Row],[DE9: VT&amp;R]]),ISBLANK(Table4[[#This Row],[DE10: multi-robot]]),ISBLANK(Table4[[#This Row],[DE11: prior]]),ISBLANK(Table4[[#This Row],[DE12: learning]]),ISBLANK(Table4[[#This Row],[DE13: computation]]),ISBLANK(Table4[[#This Row],[DE14: online/offline]]),ISBLANK(Table4[[#This Row],[DE15: environ]]),ISBLANK(Table4[[#This Row],[DE16: domain]]),ISBLANK(Table4[[#This Row],[DE17: sensor]]),ISBLANK(Table4[[#This Row],[DE18: error eval]]),ISBLANK(Table4[[#This Row],[DE19: compute eval]]),ISBLANK(Table4[[#This Row],[DE20: gt data]]),ISBLANK(Table4[[#This Row],[DE21: repo link]]),ISBLANK(Table4[[#This Row],[DE22: datasets]]),ISBLANK(Table4[[#This Row],[DE23: distance]]),ISBLANK(Table4[[#This Row],[DE24: time]])))</f>
@@ -52083,77 +52097,227 @@
         <v>1434</v>
       </c>
     </row>
-    <row r="169" spans="1:33" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:33" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A169" s="5" t="s">
-        <v>457</v>
+        <v>278</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>1697</v>
+        <v>1654</v>
       </c>
       <c r="C169" s="3">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>458</v>
+        <v>279</v>
       </c>
       <c r="E169" s="4" t="s">
-        <v>459</v>
+        <v>280</v>
+      </c>
+      <c r="F169" s="5" t="s">
+        <v>2437</v>
+      </c>
+      <c r="G169" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H169" s="5" t="s">
+        <v>2438</v>
+      </c>
+      <c r="I169" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="J169" s="5" t="s">
+        <v>2440</v>
+      </c>
+      <c r="K169" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="L169" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="M169" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="N169" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="O169" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="P169" s="5" t="s">
+        <v>2439</v>
+      </c>
+      <c r="Q169" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="R169" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="S169" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="T169" s="5" t="s">
+        <v>1399</v>
+      </c>
+      <c r="U169" s="5" t="s">
+        <v>1353</v>
+      </c>
+      <c r="V169" s="5" t="s">
+        <v>1357</v>
+      </c>
+      <c r="W169" s="5" t="s">
+        <v>2441</v>
+      </c>
+      <c r="X169" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="Y169" s="5" t="s">
+        <v>2442</v>
+      </c>
+      <c r="Z169" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="AA169" s="5" t="s">
+        <v>2445</v>
+      </c>
+      <c r="AB169" s="5" t="s">
+        <v>2443</v>
+      </c>
+      <c r="AC169" s="5" t="s">
+        <v>2444</v>
+      </c>
+      <c r="AD169" s="5" t="s">
+        <v>2446</v>
       </c>
       <c r="AE169" s="5" t="b">
         <f>NOT(OR(ISBLANK(Table4[[#This Row],[DE1: name]]),ISBLANK(Table4[[#This Row],[DE2: extended version]]),ISBLANK(Table4[[#This Row],[DE3: long-term]]),ISBLANK(Table4[[#This Row],[DE4: local+map]]),ISBLANK(Table4[[#This Row],[DE5: localizer]]),ISBLANK(Table4[[#This Row],[DE6: map]]),ISBLANK(Table4[[#This Row],[DE7: active SLAM]]),ISBLANK(Table4[[#This Row],[DE8: SPLAM]]),ISBLANK(Table4[[#This Row],[DE9: VT&amp;R]]),ISBLANK(Table4[[#This Row],[DE10: multi-robot]]),ISBLANK(Table4[[#This Row],[DE11: prior]]),ISBLANK(Table4[[#This Row],[DE12: learning]]),ISBLANK(Table4[[#This Row],[DE13: computation]]),ISBLANK(Table4[[#This Row],[DE14: online/offline]]),ISBLANK(Table4[[#This Row],[DE15: environ]]),ISBLANK(Table4[[#This Row],[DE16: domain]]),ISBLANK(Table4[[#This Row],[DE17: sensor]]),ISBLANK(Table4[[#This Row],[DE18: error eval]]),ISBLANK(Table4[[#This Row],[DE19: compute eval]]),ISBLANK(Table4[[#This Row],[DE20: gt data]]),ISBLANK(Table4[[#This Row],[DE21: repo link]]),ISBLANK(Table4[[#This Row],[DE22: datasets]]),ISBLANK(Table4[[#This Row],[DE23: distance]]),ISBLANK(Table4[[#This Row],[DE24: time]])))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF169" s="5" t="b">
         <f>AND(Table4[[#This Row],[all data?]],NOT(OR(Table4[[#This Row],[DE1: name]]="?",Table4[[#This Row],[DE2: extended version]]="?",Table4[[#This Row],[DE3: long-term]]="?",Table4[[#This Row],[DE4: local+map]]="?",Table4[[#This Row],[DE5: localizer]]="?",Table4[[#This Row],[DE6: map]]="?",Table4[[#This Row],[DE7: active SLAM]]="?",Table4[[#This Row],[DE8: SPLAM]]="?",Table4[[#This Row],[DE9: VT&amp;R]]="?",Table4[[#This Row],[DE10: multi-robot]]="?",Table4[[#This Row],[DE11: prior]]="?",Table4[[#This Row],[DE12: learning]]="?",Table4[[#This Row],[DE13: computation]]="?",Table4[[#This Row],[DE14: online/offline]]="?",Table4[[#This Row],[DE15: environ]]="?",Table4[[#This Row],[DE16: domain]]="?",Table4[[#This Row],[DE17: sensor]]="?",Table4[[#This Row],[DE18: error eval]]="?",Table4[[#This Row],[DE19: compute eval]]="?",Table4[[#This Row],[DE20: gt data]]="?",Table4[[#This Row],[DE21: repo link]]="?",Table4[[#This Row],[DE22: datasets]]="?",Table4[[#This Row],[DE23: distance]]="?",Table4[[#This Row],[DE24: time]]="?")))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG169" s="5" t="s">
         <v>1434</v>
       </c>
     </row>
-    <row r="170" spans="1:33" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:33" ht="132" x14ac:dyDescent="0.3">
       <c r="A170" s="5" t="s">
-        <v>496</v>
+        <v>335</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>1721</v>
+        <v>1670</v>
       </c>
       <c r="C170" s="3">
-        <v>2020</v>
-      </c>
-      <c r="D170" s="3" t="s">
-        <v>497</v>
+        <v>2018</v>
       </c>
       <c r="E170" s="4" t="s">
-        <v>498</v>
+        <v>336</v>
+      </c>
+      <c r="F170" s="5" t="s">
+        <v>2531</v>
+      </c>
+      <c r="G170" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="H170" s="5" t="s">
+        <v>2549</v>
+      </c>
+      <c r="I170" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="J170" s="5" t="s">
+        <v>2551</v>
+      </c>
+      <c r="K170" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="L170" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="M170" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="N170" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="O170" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="P170" s="5" t="s">
+        <v>655</v>
+      </c>
+      <c r="Q170" s="5" t="s">
+        <v>2550</v>
+      </c>
+      <c r="R170" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="S170" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="T170" s="5" t="s">
+        <v>1399</v>
+      </c>
+      <c r="U170" s="5" t="s">
+        <v>1353</v>
+      </c>
+      <c r="V170" s="5" t="s">
+        <v>1357</v>
+      </c>
+      <c r="W170" s="5" t="s">
+        <v>1536</v>
+      </c>
+      <c r="X170" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="Y170" s="5" t="s">
+        <v>2538</v>
+      </c>
+      <c r="Z170" s="5" t="s">
+        <v>1342</v>
+      </c>
+      <c r="AA170" s="5" t="s">
+        <v>2534</v>
+      </c>
+      <c r="AB170" s="5" t="s">
+        <v>2536</v>
+      </c>
+      <c r="AC170" s="5" t="s">
+        <v>2537</v>
+      </c>
+      <c r="AD170" s="5" t="s">
+        <v>1342</v>
       </c>
       <c r="AE170" s="5" t="b">
         <f>NOT(OR(ISBLANK(Table4[[#This Row],[DE1: name]]),ISBLANK(Table4[[#This Row],[DE2: extended version]]),ISBLANK(Table4[[#This Row],[DE3: long-term]]),ISBLANK(Table4[[#This Row],[DE4: local+map]]),ISBLANK(Table4[[#This Row],[DE5: localizer]]),ISBLANK(Table4[[#This Row],[DE6: map]]),ISBLANK(Table4[[#This Row],[DE7: active SLAM]]),ISBLANK(Table4[[#This Row],[DE8: SPLAM]]),ISBLANK(Table4[[#This Row],[DE9: VT&amp;R]]),ISBLANK(Table4[[#This Row],[DE10: multi-robot]]),ISBLANK(Table4[[#This Row],[DE11: prior]]),ISBLANK(Table4[[#This Row],[DE12: learning]]),ISBLANK(Table4[[#This Row],[DE13: computation]]),ISBLANK(Table4[[#This Row],[DE14: online/offline]]),ISBLANK(Table4[[#This Row],[DE15: environ]]),ISBLANK(Table4[[#This Row],[DE16: domain]]),ISBLANK(Table4[[#This Row],[DE17: sensor]]),ISBLANK(Table4[[#This Row],[DE18: error eval]]),ISBLANK(Table4[[#This Row],[DE19: compute eval]]),ISBLANK(Table4[[#This Row],[DE20: gt data]]),ISBLANK(Table4[[#This Row],[DE21: repo link]]),ISBLANK(Table4[[#This Row],[DE22: datasets]]),ISBLANK(Table4[[#This Row],[DE23: distance]]),ISBLANK(Table4[[#This Row],[DE24: time]])))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF170" s="5" t="b">
         <f>AND(Table4[[#This Row],[all data?]],NOT(OR(Table4[[#This Row],[DE1: name]]="?",Table4[[#This Row],[DE2: extended version]]="?",Table4[[#This Row],[DE3: long-term]]="?",Table4[[#This Row],[DE4: local+map]]="?",Table4[[#This Row],[DE5: localizer]]="?",Table4[[#This Row],[DE6: map]]="?",Table4[[#This Row],[DE7: active SLAM]]="?",Table4[[#This Row],[DE8: SPLAM]]="?",Table4[[#This Row],[DE9: VT&amp;R]]="?",Table4[[#This Row],[DE10: multi-robot]]="?",Table4[[#This Row],[DE11: prior]]="?",Table4[[#This Row],[DE12: learning]]="?",Table4[[#This Row],[DE13: computation]]="?",Table4[[#This Row],[DE14: online/offline]]="?",Table4[[#This Row],[DE15: environ]]="?",Table4[[#This Row],[DE16: domain]]="?",Table4[[#This Row],[DE17: sensor]]="?",Table4[[#This Row],[DE18: error eval]]="?",Table4[[#This Row],[DE19: compute eval]]="?",Table4[[#This Row],[DE20: gt data]]="?",Table4[[#This Row],[DE21: repo link]]="?",Table4[[#This Row],[DE22: datasets]]="?",Table4[[#This Row],[DE23: distance]]="?",Table4[[#This Row],[DE24: time]]="?")))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG170" s="5" t="s">
         <v>1434</v>
       </c>
     </row>
-    <row r="171" spans="1:33" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:33" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A171" s="5" t="s">
-        <v>564</v>
+        <v>346</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>1742</v>
+        <v>1600</v>
       </c>
       <c r="C171" s="3">
-        <v>2021</v>
+        <v>2018</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>565</v>
+        <v>347</v>
       </c>
       <c r="E171" s="4" t="s">
-        <v>566</v>
+        <v>348</v>
+      </c>
+      <c r="F171" s="5" t="s">
+        <v>1532</v>
       </c>
       <c r="AE171" s="5" t="b">
         <f>NOT(OR(ISBLANK(Table4[[#This Row],[DE1: name]]),ISBLANK(Table4[[#This Row],[DE2: extended version]]),ISBLANK(Table4[[#This Row],[DE3: long-term]]),ISBLANK(Table4[[#This Row],[DE4: local+map]]),ISBLANK(Table4[[#This Row],[DE5: localizer]]),ISBLANK(Table4[[#This Row],[DE6: map]]),ISBLANK(Table4[[#This Row],[DE7: active SLAM]]),ISBLANK(Table4[[#This Row],[DE8: SPLAM]]),ISBLANK(Table4[[#This Row],[DE9: VT&amp;R]]),ISBLANK(Table4[[#This Row],[DE10: multi-robot]]),ISBLANK(Table4[[#This Row],[DE11: prior]]),ISBLANK(Table4[[#This Row],[DE12: learning]]),ISBLANK(Table4[[#This Row],[DE13: computation]]),ISBLANK(Table4[[#This Row],[DE14: online/offline]]),ISBLANK(Table4[[#This Row],[DE15: environ]]),ISBLANK(Table4[[#This Row],[DE16: domain]]),ISBLANK(Table4[[#This Row],[DE17: sensor]]),ISBLANK(Table4[[#This Row],[DE18: error eval]]),ISBLANK(Table4[[#This Row],[DE19: compute eval]]),ISBLANK(Table4[[#This Row],[DE20: gt data]]),ISBLANK(Table4[[#This Row],[DE21: repo link]]),ISBLANK(Table4[[#This Row],[DE22: datasets]]),ISBLANK(Table4[[#This Row],[DE23: distance]]),ISBLANK(Table4[[#This Row],[DE24: time]])))</f>
@@ -52164,236 +52328,80 @@
         <v>0</v>
       </c>
       <c r="AG171" s="5" t="s">
-        <v>1434</v>
-      </c>
-    </row>
-    <row r="172" spans="1:33" ht="105.6" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="172" spans="1:33" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A172" s="5" t="s">
-        <v>92</v>
+        <v>349</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>1602</v>
+        <v>1674</v>
       </c>
       <c r="C172" s="3">
-        <v>2011</v>
+        <v>2018</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>93</v>
+        <v>350</v>
       </c>
       <c r="E172" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="F172" s="5" t="s">
-        <v>1543</v>
-      </c>
-      <c r="G172" s="5" t="s">
-        <v>1542</v>
-      </c>
-      <c r="H172" s="5" t="s">
-        <v>1547</v>
-      </c>
-      <c r="I172" s="5" t="s">
-        <v>1386</v>
-      </c>
-      <c r="J172" s="5" t="s">
-        <v>1484</v>
-      </c>
-      <c r="K172" s="5" t="s">
-        <v>2012</v>
-      </c>
-      <c r="L172" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="M172" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="N172" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="O172" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="P172" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="Q172" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="R172" s="5" t="s">
-        <v>1349</v>
-      </c>
-      <c r="S172" s="5" t="s">
-        <v>1351</v>
-      </c>
-      <c r="T172" s="5" t="s">
-        <v>1548</v>
-      </c>
-      <c r="U172" s="5" t="s">
-        <v>1353</v>
-      </c>
-      <c r="V172" s="5" t="s">
-        <v>1481</v>
-      </c>
-      <c r="W172" s="5" t="s">
-        <v>1550</v>
-      </c>
-      <c r="X172" s="5" t="s">
-        <v>1549</v>
-      </c>
-      <c r="Y172" s="5" t="s">
-        <v>1551</v>
-      </c>
-      <c r="Z172" s="5" t="s">
-        <v>1342</v>
-      </c>
-      <c r="AA172" s="5" t="s">
-        <v>1552</v>
-      </c>
-      <c r="AB172" s="5" t="s">
-        <v>1342</v>
-      </c>
-      <c r="AC172" s="5" t="s">
-        <v>1342</v>
-      </c>
-      <c r="AD172" s="5" t="s">
-        <v>1546</v>
+        <v>351</v>
       </c>
       <c r="AE172" s="5" t="b">
         <f>NOT(OR(ISBLANK(Table4[[#This Row],[DE1: name]]),ISBLANK(Table4[[#This Row],[DE2: extended version]]),ISBLANK(Table4[[#This Row],[DE3: long-term]]),ISBLANK(Table4[[#This Row],[DE4: local+map]]),ISBLANK(Table4[[#This Row],[DE5: localizer]]),ISBLANK(Table4[[#This Row],[DE6: map]]),ISBLANK(Table4[[#This Row],[DE7: active SLAM]]),ISBLANK(Table4[[#This Row],[DE8: SPLAM]]),ISBLANK(Table4[[#This Row],[DE9: VT&amp;R]]),ISBLANK(Table4[[#This Row],[DE10: multi-robot]]),ISBLANK(Table4[[#This Row],[DE11: prior]]),ISBLANK(Table4[[#This Row],[DE12: learning]]),ISBLANK(Table4[[#This Row],[DE13: computation]]),ISBLANK(Table4[[#This Row],[DE14: online/offline]]),ISBLANK(Table4[[#This Row],[DE15: environ]]),ISBLANK(Table4[[#This Row],[DE16: domain]]),ISBLANK(Table4[[#This Row],[DE17: sensor]]),ISBLANK(Table4[[#This Row],[DE18: error eval]]),ISBLANK(Table4[[#This Row],[DE19: compute eval]]),ISBLANK(Table4[[#This Row],[DE20: gt data]]),ISBLANK(Table4[[#This Row],[DE21: repo link]]),ISBLANK(Table4[[#This Row],[DE22: datasets]]),ISBLANK(Table4[[#This Row],[DE23: distance]]),ISBLANK(Table4[[#This Row],[DE24: time]])))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF172" s="5" t="b">
         <f>AND(Table4[[#This Row],[all data?]],NOT(OR(Table4[[#This Row],[DE1: name]]="?",Table4[[#This Row],[DE2: extended version]]="?",Table4[[#This Row],[DE3: long-term]]="?",Table4[[#This Row],[DE4: local+map]]="?",Table4[[#This Row],[DE5: localizer]]="?",Table4[[#This Row],[DE6: map]]="?",Table4[[#This Row],[DE7: active SLAM]]="?",Table4[[#This Row],[DE8: SPLAM]]="?",Table4[[#This Row],[DE9: VT&amp;R]]="?",Table4[[#This Row],[DE10: multi-robot]]="?",Table4[[#This Row],[DE11: prior]]="?",Table4[[#This Row],[DE12: learning]]="?",Table4[[#This Row],[DE13: computation]]="?",Table4[[#This Row],[DE14: online/offline]]="?",Table4[[#This Row],[DE15: environ]]="?",Table4[[#This Row],[DE16: domain]]="?",Table4[[#This Row],[DE17: sensor]]="?",Table4[[#This Row],[DE18: error eval]]="?",Table4[[#This Row],[DE19: compute eval]]="?",Table4[[#This Row],[DE20: gt data]]="?",Table4[[#This Row],[DE21: repo link]]="?",Table4[[#This Row],[DE22: datasets]]="?",Table4[[#This Row],[DE23: distance]]="?",Table4[[#This Row],[DE24: time]]="?")))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG172" s="5" t="s">
-        <v>2001</v>
-      </c>
-    </row>
-    <row r="173" spans="1:33" ht="184.8" x14ac:dyDescent="0.3">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="173" spans="1:33" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A173" s="5" t="s">
-        <v>86</v>
+        <v>424</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>1600</v>
+        <v>1699</v>
       </c>
       <c r="C173" s="3">
-        <v>2011</v>
+        <v>2019</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>87</v>
+        <v>425</v>
       </c>
       <c r="E173" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="F173" s="5" t="s">
-        <v>1532</v>
-      </c>
-      <c r="G173" s="5" t="s">
-        <v>1342</v>
-      </c>
-      <c r="H173" s="5" t="s">
-        <v>1533</v>
-      </c>
-      <c r="I173" s="5" t="s">
-        <v>1386</v>
-      </c>
-      <c r="J173" s="5" t="s">
-        <v>1535</v>
-      </c>
-      <c r="K173" s="5" t="s">
-        <v>1534</v>
-      </c>
-      <c r="L173" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="M173" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="N173" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="O173" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="P173" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="Q173" s="5" t="s">
-        <v>655</v>
-      </c>
-      <c r="R173" s="5" t="s">
-        <v>1349</v>
-      </c>
-      <c r="S173" s="5" t="s">
-        <v>1351</v>
-      </c>
-      <c r="T173" s="5" t="s">
-        <v>1399</v>
-      </c>
-      <c r="U173" s="5" t="s">
-        <v>1353</v>
-      </c>
-      <c r="V173" s="5" t="s">
-        <v>1357</v>
-      </c>
-      <c r="W173" s="5" t="s">
-        <v>1536</v>
-      </c>
-      <c r="X173" s="5" t="s">
-        <v>1537</v>
-      </c>
-      <c r="Y173" s="5" t="s">
-        <v>1538</v>
-      </c>
-      <c r="Z173" s="5" t="s">
-        <v>1539</v>
-      </c>
-      <c r="AA173" s="5" t="s">
-        <v>1540</v>
-      </c>
-      <c r="AB173" s="5" t="s">
-        <v>1342</v>
-      </c>
-      <c r="AC173" s="5" t="s">
-        <v>1342</v>
-      </c>
-      <c r="AD173" s="5" t="s">
-        <v>1342</v>
+        <v>426</v>
       </c>
       <c r="AE173" s="5" t="b">
         <f>NOT(OR(ISBLANK(Table4[[#This Row],[DE1: name]]),ISBLANK(Table4[[#This Row],[DE2: extended version]]),ISBLANK(Table4[[#This Row],[DE3: long-term]]),ISBLANK(Table4[[#This Row],[DE4: local+map]]),ISBLANK(Table4[[#This Row],[DE5: localizer]]),ISBLANK(Table4[[#This Row],[DE6: map]]),ISBLANK(Table4[[#This Row],[DE7: active SLAM]]),ISBLANK(Table4[[#This Row],[DE8: SPLAM]]),ISBLANK(Table4[[#This Row],[DE9: VT&amp;R]]),ISBLANK(Table4[[#This Row],[DE10: multi-robot]]),ISBLANK(Table4[[#This Row],[DE11: prior]]),ISBLANK(Table4[[#This Row],[DE12: learning]]),ISBLANK(Table4[[#This Row],[DE13: computation]]),ISBLANK(Table4[[#This Row],[DE14: online/offline]]),ISBLANK(Table4[[#This Row],[DE15: environ]]),ISBLANK(Table4[[#This Row],[DE16: domain]]),ISBLANK(Table4[[#This Row],[DE17: sensor]]),ISBLANK(Table4[[#This Row],[DE18: error eval]]),ISBLANK(Table4[[#This Row],[DE19: compute eval]]),ISBLANK(Table4[[#This Row],[DE20: gt data]]),ISBLANK(Table4[[#This Row],[DE21: repo link]]),ISBLANK(Table4[[#This Row],[DE22: datasets]]),ISBLANK(Table4[[#This Row],[DE23: distance]]),ISBLANK(Table4[[#This Row],[DE24: time]])))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF173" s="5" t="b">
         <f>AND(Table4[[#This Row],[all data?]],NOT(OR(Table4[[#This Row],[DE1: name]]="?",Table4[[#This Row],[DE2: extended version]]="?",Table4[[#This Row],[DE3: long-term]]="?",Table4[[#This Row],[DE4: local+map]]="?",Table4[[#This Row],[DE5: localizer]]="?",Table4[[#This Row],[DE6: map]]="?",Table4[[#This Row],[DE7: active SLAM]]="?",Table4[[#This Row],[DE8: SPLAM]]="?",Table4[[#This Row],[DE9: VT&amp;R]]="?",Table4[[#This Row],[DE10: multi-robot]]="?",Table4[[#This Row],[DE11: prior]]="?",Table4[[#This Row],[DE12: learning]]="?",Table4[[#This Row],[DE13: computation]]="?",Table4[[#This Row],[DE14: online/offline]]="?",Table4[[#This Row],[DE15: environ]]="?",Table4[[#This Row],[DE16: domain]]="?",Table4[[#This Row],[DE17: sensor]]="?",Table4[[#This Row],[DE18: error eval]]="?",Table4[[#This Row],[DE19: compute eval]]="?",Table4[[#This Row],[DE20: gt data]]="?",Table4[[#This Row],[DE21: repo link]]="?",Table4[[#This Row],[DE22: datasets]]="?",Table4[[#This Row],[DE23: distance]]="?",Table4[[#This Row],[DE24: time]]="?")))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG173" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="174" spans="1:33" ht="39.6" x14ac:dyDescent="0.3">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="174" spans="1:33" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A174" s="5" t="s">
-        <v>89</v>
+        <v>457</v>
       </c>
       <c r="B174" s="3" t="s">
-        <v>1601</v>
+        <v>1697</v>
       </c>
       <c r="C174" s="3">
-        <v>2011</v>
+        <v>2019</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>90</v>
+        <v>458</v>
       </c>
       <c r="E174" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F174" s="5" t="s">
-        <v>1545</v>
-      </c>
-      <c r="G174" s="5" t="s">
-        <v>1541</v>
+        <v>459</v>
       </c>
       <c r="AE174" s="5" t="b">
         <f>NOT(OR(ISBLANK(Table4[[#This Row],[DE1: name]]),ISBLANK(Table4[[#This Row],[DE2: extended version]]),ISBLANK(Table4[[#This Row],[DE3: long-term]]),ISBLANK(Table4[[#This Row],[DE4: local+map]]),ISBLANK(Table4[[#This Row],[DE5: localizer]]),ISBLANK(Table4[[#This Row],[DE6: map]]),ISBLANK(Table4[[#This Row],[DE7: active SLAM]]),ISBLANK(Table4[[#This Row],[DE8: SPLAM]]),ISBLANK(Table4[[#This Row],[DE9: VT&amp;R]]),ISBLANK(Table4[[#This Row],[DE10: multi-robot]]),ISBLANK(Table4[[#This Row],[DE11: prior]]),ISBLANK(Table4[[#This Row],[DE12: learning]]),ISBLANK(Table4[[#This Row],[DE13: computation]]),ISBLANK(Table4[[#This Row],[DE14: online/offline]]),ISBLANK(Table4[[#This Row],[DE15: environ]]),ISBLANK(Table4[[#This Row],[DE16: domain]]),ISBLANK(Table4[[#This Row],[DE17: sensor]]),ISBLANK(Table4[[#This Row],[DE18: error eval]]),ISBLANK(Table4[[#This Row],[DE19: compute eval]]),ISBLANK(Table4[[#This Row],[DE20: gt data]]),ISBLANK(Table4[[#This Row],[DE21: repo link]]),ISBLANK(Table4[[#This Row],[DE22: datasets]]),ISBLANK(Table4[[#This Row],[DE23: distance]]),ISBLANK(Table4[[#This Row],[DE24: time]])))</f>
@@ -52404,27 +52412,24 @@
         <v>0</v>
       </c>
       <c r="AG174" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="175" spans="1:33" ht="26.4" x14ac:dyDescent="0.3">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="175" spans="1:33" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A175" s="5" t="s">
-        <v>128</v>
+        <v>496</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>1611</v>
+        <v>1721</v>
       </c>
       <c r="C175" s="3">
-        <v>2013</v>
+        <v>2020</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>129</v>
+        <v>497</v>
       </c>
       <c r="E175" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="F175" s="5" t="s">
-        <v>1532</v>
+        <v>498</v>
       </c>
       <c r="AE175" s="5" t="b">
         <f>NOT(OR(ISBLANK(Table4[[#This Row],[DE1: name]]),ISBLANK(Table4[[#This Row],[DE2: extended version]]),ISBLANK(Table4[[#This Row],[DE3: long-term]]),ISBLANK(Table4[[#This Row],[DE4: local+map]]),ISBLANK(Table4[[#This Row],[DE5: localizer]]),ISBLANK(Table4[[#This Row],[DE6: map]]),ISBLANK(Table4[[#This Row],[DE7: active SLAM]]),ISBLANK(Table4[[#This Row],[DE8: SPLAM]]),ISBLANK(Table4[[#This Row],[DE9: VT&amp;R]]),ISBLANK(Table4[[#This Row],[DE10: multi-robot]]),ISBLANK(Table4[[#This Row],[DE11: prior]]),ISBLANK(Table4[[#This Row],[DE12: learning]]),ISBLANK(Table4[[#This Row],[DE13: computation]]),ISBLANK(Table4[[#This Row],[DE14: online/offline]]),ISBLANK(Table4[[#This Row],[DE15: environ]]),ISBLANK(Table4[[#This Row],[DE16: domain]]),ISBLANK(Table4[[#This Row],[DE17: sensor]]),ISBLANK(Table4[[#This Row],[DE18: error eval]]),ISBLANK(Table4[[#This Row],[DE19: compute eval]]),ISBLANK(Table4[[#This Row],[DE20: gt data]]),ISBLANK(Table4[[#This Row],[DE21: repo link]]),ISBLANK(Table4[[#This Row],[DE22: datasets]]),ISBLANK(Table4[[#This Row],[DE23: distance]]),ISBLANK(Table4[[#This Row],[DE24: time]])))</f>
@@ -52435,27 +52440,24 @@
         <v>0</v>
       </c>
       <c r="AG175" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="176" spans="1:33" ht="26.4" x14ac:dyDescent="0.3">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="176" spans="1:33" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A176" s="5" t="s">
-        <v>346</v>
+        <v>564</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>1600</v>
+        <v>1742</v>
       </c>
       <c r="C176" s="3">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>347</v>
+        <v>565</v>
       </c>
       <c r="E176" s="4" t="s">
-        <v>348</v>
-      </c>
-      <c r="F176" s="5" t="s">
-        <v>1532</v>
+        <v>566</v>
       </c>
       <c r="AE176" s="5" t="b">
         <f>NOT(OR(ISBLANK(Table4[[#This Row],[DE1: name]]),ISBLANK(Table4[[#This Row],[DE2: extended version]]),ISBLANK(Table4[[#This Row],[DE3: long-term]]),ISBLANK(Table4[[#This Row],[DE4: local+map]]),ISBLANK(Table4[[#This Row],[DE5: localizer]]),ISBLANK(Table4[[#This Row],[DE6: map]]),ISBLANK(Table4[[#This Row],[DE7: active SLAM]]),ISBLANK(Table4[[#This Row],[DE8: SPLAM]]),ISBLANK(Table4[[#This Row],[DE9: VT&amp;R]]),ISBLANK(Table4[[#This Row],[DE10: multi-robot]]),ISBLANK(Table4[[#This Row],[DE11: prior]]),ISBLANK(Table4[[#This Row],[DE12: learning]]),ISBLANK(Table4[[#This Row],[DE13: computation]]),ISBLANK(Table4[[#This Row],[DE14: online/offline]]),ISBLANK(Table4[[#This Row],[DE15: environ]]),ISBLANK(Table4[[#This Row],[DE16: domain]]),ISBLANK(Table4[[#This Row],[DE17: sensor]]),ISBLANK(Table4[[#This Row],[DE18: error eval]]),ISBLANK(Table4[[#This Row],[DE19: compute eval]]),ISBLANK(Table4[[#This Row],[DE20: gt data]]),ISBLANK(Table4[[#This Row],[DE21: repo link]]),ISBLANK(Table4[[#This Row],[DE22: datasets]]),ISBLANK(Table4[[#This Row],[DE23: distance]]),ISBLANK(Table4[[#This Row],[DE24: time]])))</f>
@@ -52466,7 +52468,7 @@
         <v>0</v>
       </c>
       <c r="AG176" s="5" t="s">
-        <v>23</v>
+        <v>1434</v>
       </c>
     </row>
   </sheetData>
@@ -52797,25 +52799,25 @@
     <hyperlink ref="E147" r:id="rId3" xr:uid="{DAE3E679-F97A-4190-AD29-37D285FABD93}"/>
     <hyperlink ref="E4" r:id="rId4" xr:uid="{DC01640B-4C83-4F19-B485-86FC177CD84D}"/>
     <hyperlink ref="E5" r:id="rId5" xr:uid="{CE8FD8F2-EDAD-44E3-B25C-2F626F99E710}"/>
-    <hyperlink ref="E150" r:id="rId6" xr:uid="{DAA2868F-9677-45ED-90EF-F2508774C75B}"/>
+    <hyperlink ref="E148" r:id="rId6" xr:uid="{DAA2868F-9677-45ED-90EF-F2508774C75B}"/>
     <hyperlink ref="E6" r:id="rId7" xr:uid="{B63DB040-7E79-4180-A7B1-8967CB7B17E6}"/>
     <hyperlink ref="E7" r:id="rId8" xr:uid="{7356C955-9DE3-4773-B770-EC935E099792}"/>
     <hyperlink ref="E8" r:id="rId9" xr:uid="{29F4EA37-3E90-443A-B1CF-136DDB974F18}"/>
     <hyperlink ref="E9" r:id="rId10" xr:uid="{A9F7C589-6B92-4AA5-B0AA-AB9A7C52026A}"/>
-    <hyperlink ref="E148" r:id="rId11" xr:uid="{C1E7D7C8-9398-4CE9-A428-6F901474B1EC}"/>
+    <hyperlink ref="E149" r:id="rId11" xr:uid="{C1E7D7C8-9398-4CE9-A428-6F901474B1EC}"/>
     <hyperlink ref="E10" r:id="rId12" xr:uid="{4EA53226-0BAD-40CF-B5E9-4344C6F106AC}"/>
     <hyperlink ref="E11" r:id="rId13" xr:uid="{4C9DA339-E509-4A4C-8D50-C3226501D04D}"/>
-    <hyperlink ref="E149" r:id="rId14" xr:uid="{A9EEEB0B-4677-4D6A-95C9-CD5CAC60160C}"/>
+    <hyperlink ref="E150" r:id="rId14" xr:uid="{A9EEEB0B-4677-4D6A-95C9-CD5CAC60160C}"/>
     <hyperlink ref="E12" r:id="rId15" xr:uid="{C54CD96C-E0F9-44D9-A925-ABA4C51B2297}"/>
     <hyperlink ref="E13" r:id="rId16" xr:uid="{F2CDCEDD-2471-44D4-9A59-5BA10FE7FE91}"/>
     <hyperlink ref="E151" r:id="rId17" xr:uid="{600230A1-8932-4767-AFCB-D9D368391314}"/>
     <hyperlink ref="E14" r:id="rId18" xr:uid="{2599D912-4165-4663-ACD2-E64CA9F7B7E5}"/>
     <hyperlink ref="E15" r:id="rId19" xr:uid="{2F806194-81FA-45B4-9438-02C1D7F9EBE4}"/>
     <hyperlink ref="E16" r:id="rId20" xr:uid="{E7E66D97-44B8-441A-A585-2514E51497CE}"/>
-    <hyperlink ref="E173" r:id="rId21" xr:uid="{31F2CD4D-8F00-4493-A41A-0D1634D5624D}"/>
-    <hyperlink ref="E174" r:id="rId22" xr:uid="{708E9554-CB81-4E36-BCA3-0F971B1C7EC4}"/>
-    <hyperlink ref="E172" r:id="rId23" xr:uid="{03E1C5BE-72CC-46AF-92D8-13C8E40D5CDC}"/>
-    <hyperlink ref="E152" r:id="rId24" xr:uid="{919AC5BE-9928-439B-A1FF-BCF354BAA8AD}"/>
+    <hyperlink ref="E152" r:id="rId21" xr:uid="{31F2CD4D-8F00-4493-A41A-0D1634D5624D}"/>
+    <hyperlink ref="E153" r:id="rId22" xr:uid="{708E9554-CB81-4E36-BCA3-0F971B1C7EC4}"/>
+    <hyperlink ref="E154" r:id="rId23" xr:uid="{03E1C5BE-72CC-46AF-92D8-13C8E40D5CDC}"/>
+    <hyperlink ref="E155" r:id="rId24" xr:uid="{919AC5BE-9928-439B-A1FF-BCF354BAA8AD}"/>
     <hyperlink ref="E17" r:id="rId25" xr:uid="{415779DE-5051-4AA9-B9C0-B47BCFB5C2CC}"/>
     <hyperlink ref="E18" r:id="rId26" xr:uid="{1D9CDEE8-8DCB-4303-9F3B-D2E39307B539}"/>
     <hyperlink ref="E19" r:id="rId27" xr:uid="{7F8B1295-B2EB-4944-A0AF-73192C8647B8}"/>
@@ -52823,8 +52825,8 @@
     <hyperlink ref="E21" r:id="rId29" xr:uid="{B215C7F4-F9F7-4770-96A0-EF34818D77B1}"/>
     <hyperlink ref="E22" r:id="rId30" xr:uid="{F0DD0C95-5BEC-47FB-8D70-E9AD2598C55B}"/>
     <hyperlink ref="E23" r:id="rId31" xr:uid="{6AD21EC9-459A-4D97-8B9B-D21A8B857931}"/>
-    <hyperlink ref="E153" r:id="rId32" xr:uid="{104E4037-D3F1-4BC3-847D-7D0839164079}"/>
-    <hyperlink ref="E175" r:id="rId33" xr:uid="{90CA1D91-47FB-4131-8F34-F424A5862383}"/>
+    <hyperlink ref="E156" r:id="rId32" xr:uid="{104E4037-D3F1-4BC3-847D-7D0839164079}"/>
+    <hyperlink ref="E157" r:id="rId33" xr:uid="{90CA1D91-47FB-4131-8F34-F424A5862383}"/>
     <hyperlink ref="E24" r:id="rId34" xr:uid="{D133BA6C-6061-4A03-A555-160078908970}"/>
     <hyperlink ref="E25" r:id="rId35" xr:uid="{A5309F62-5B9B-4C6C-9DB7-6B9940D222BA}"/>
     <hyperlink ref="E26" r:id="rId36" xr:uid="{ABBF501C-BD20-4E9F-B0EE-FDB0E32B78C8}"/>
@@ -52832,19 +52834,19 @@
     <hyperlink ref="E28" r:id="rId38" xr:uid="{59B9E4A3-6EDD-4E8A-A336-D76F84909946}"/>
     <hyperlink ref="E29" r:id="rId39" xr:uid="{37AFCAC2-FA5F-45EC-A069-44B7A4EBFACC}"/>
     <hyperlink ref="E30" r:id="rId40" xr:uid="{CBAA50C7-09F8-4069-A6CF-6685A317D83A}"/>
-    <hyperlink ref="E154" r:id="rId41" xr:uid="{8DDE7B23-2D52-4DF7-8FE2-80BFE2E7DC6C}"/>
+    <hyperlink ref="E158" r:id="rId41" xr:uid="{8DDE7B23-2D52-4DF7-8FE2-80BFE2E7DC6C}"/>
     <hyperlink ref="E31" r:id="rId42" xr:uid="{12E4E2AA-1C6A-4403-8C5C-5C8D9857EA03}"/>
-    <hyperlink ref="E155" r:id="rId43" xr:uid="{F0238F49-1995-46A0-9792-0D504795CA32}"/>
-    <hyperlink ref="E156" r:id="rId44" xr:uid="{EA18EB4C-5A13-48A0-AC20-A4111FCF8C16}"/>
+    <hyperlink ref="E159" r:id="rId43" xr:uid="{F0238F49-1995-46A0-9792-0D504795CA32}"/>
+    <hyperlink ref="E160" r:id="rId44" xr:uid="{EA18EB4C-5A13-48A0-AC20-A4111FCF8C16}"/>
     <hyperlink ref="E32" r:id="rId45" xr:uid="{DE404345-384E-40D5-A36A-D216E6B93215}"/>
     <hyperlink ref="E33" r:id="rId46" xr:uid="{19190A0E-FD64-466C-AF4C-C89772C75918}"/>
     <hyperlink ref="E34" r:id="rId47" xr:uid="{35E65AF1-DECB-47F5-A633-8BB77977C832}"/>
     <hyperlink ref="E35" r:id="rId48" xr:uid="{D610D97B-8506-47AF-93BA-A63619ADE01B}"/>
-    <hyperlink ref="E157" r:id="rId49" xr:uid="{153E3F53-93C5-4F06-8F3E-7FA2D0856AFD}"/>
+    <hyperlink ref="E161" r:id="rId49" xr:uid="{153E3F53-93C5-4F06-8F3E-7FA2D0856AFD}"/>
     <hyperlink ref="E36" r:id="rId50" xr:uid="{202661FC-EDAF-4114-88E4-0238EF4D26D1}"/>
     <hyperlink ref="E37" r:id="rId51" xr:uid="{E99185F2-4D86-49BD-94BE-9A5E52A68C70}"/>
     <hyperlink ref="E38" r:id="rId52" xr:uid="{DC15C080-63D0-4F1A-8CB2-F9B179483FCC}"/>
-    <hyperlink ref="E158" r:id="rId53" xr:uid="{268EE675-604F-41B5-BC07-4BFFD34A10FB}"/>
+    <hyperlink ref="E162" r:id="rId53" xr:uid="{268EE675-604F-41B5-BC07-4BFFD34A10FB}"/>
     <hyperlink ref="E39" r:id="rId54" xr:uid="{66AD939E-C741-4F12-A136-660552A3D3F5}"/>
     <hyperlink ref="E40" r:id="rId55" xr:uid="{EF268706-06A3-4B71-9A48-E5C5DD8DA8F5}"/>
     <hyperlink ref="E41" r:id="rId56" xr:uid="{F2D1561C-A340-4B68-9CED-B7FD56060B6D}"/>
@@ -52854,12 +52856,12 @@
     <hyperlink ref="E45" r:id="rId60" xr:uid="{25493019-F907-4BA5-A5D0-E398999FFA91}"/>
     <hyperlink ref="E46" r:id="rId61" xr:uid="{80AD3BF1-A67B-4EBD-9902-4BB9F526B53C}"/>
     <hyperlink ref="E47" r:id="rId62" xr:uid="{6F3812F3-53D7-43CA-99CC-362E8CDB39F2}"/>
-    <hyperlink ref="E159" r:id="rId63" xr:uid="{C1C7DA3F-641D-49AD-A2E5-16991C43346B}"/>
+    <hyperlink ref="E163" r:id="rId63" xr:uid="{C1C7DA3F-641D-49AD-A2E5-16991C43346B}"/>
     <hyperlink ref="E48" r:id="rId64" xr:uid="{052E2862-FF01-4F90-A6EB-36131533EB35}"/>
-    <hyperlink ref="E160" r:id="rId65" xr:uid="{F8C21F18-5AC2-47D5-897A-4C14B23271C1}"/>
+    <hyperlink ref="E164" r:id="rId65" xr:uid="{F8C21F18-5AC2-47D5-897A-4C14B23271C1}"/>
     <hyperlink ref="E49" r:id="rId66" xr:uid="{B5E09C99-7770-454F-AB57-6742E13B594D}"/>
-    <hyperlink ref="E161" r:id="rId67" xr:uid="{3BE3B32B-8B13-4503-B666-37075EC8B25F}"/>
-    <hyperlink ref="E162" r:id="rId68" xr:uid="{993780B7-49F2-4BBD-8B55-B3F1ADBC07AA}"/>
+    <hyperlink ref="E165" r:id="rId67" xr:uid="{3BE3B32B-8B13-4503-B666-37075EC8B25F}"/>
+    <hyperlink ref="E166" r:id="rId68" xr:uid="{993780B7-49F2-4BBD-8B55-B3F1ADBC07AA}"/>
     <hyperlink ref="E50" r:id="rId69" xr:uid="{93E997BB-9275-4784-A13C-B403F94529DF}"/>
     <hyperlink ref="E51" r:id="rId70" xr:uid="{40E3D472-EDB6-4B05-B76F-119949ABC953}"/>
     <hyperlink ref="E52" r:id="rId71" xr:uid="{633D1B5A-72A3-493D-8102-6D705774633F}"/>
@@ -52867,9 +52869,9 @@
     <hyperlink ref="E54" r:id="rId73" xr:uid="{5D56567B-38B3-4B94-B7E0-57C15981DE0D}"/>
     <hyperlink ref="E55" r:id="rId74" xr:uid="{AC89B3A7-9C3C-4242-B0B3-3401DB00B45B}"/>
     <hyperlink ref="E56" r:id="rId75" xr:uid="{1E090786-A6C6-4029-8414-9A994EF006CC}"/>
-    <hyperlink ref="E163" r:id="rId76" xr:uid="{82CDBD7D-B7AA-43B5-82AF-185A2EB87E55}"/>
-    <hyperlink ref="E164" r:id="rId77" xr:uid="{E5AF632C-375B-47F6-918E-E9B936023F82}"/>
-    <hyperlink ref="E165" r:id="rId78" xr:uid="{4E075241-5109-49E5-AF8C-E302CCAA8AE4}"/>
+    <hyperlink ref="E167" r:id="rId76" xr:uid="{82CDBD7D-B7AA-43B5-82AF-185A2EB87E55}"/>
+    <hyperlink ref="E168" r:id="rId77" xr:uid="{E5AF632C-375B-47F6-918E-E9B936023F82}"/>
+    <hyperlink ref="E169" r:id="rId78" xr:uid="{4E075241-5109-49E5-AF8C-E302CCAA8AE4}"/>
     <hyperlink ref="E57" r:id="rId79" xr:uid="{830DB3C5-5699-4543-A234-C7ED28DDA20D}"/>
     <hyperlink ref="E58" r:id="rId80" xr:uid="{F9E97433-DDAE-4BA5-8B5D-C93761549CFE}"/>
     <hyperlink ref="E59" r:id="rId81" xr:uid="{BC8BC0C1-D2EF-45E6-993A-2B93D69A2351}"/>
@@ -52886,12 +52888,12 @@
     <hyperlink ref="E70" r:id="rId92" xr:uid="{A79FA5FD-969F-4898-BB39-F6F9D02A631D}"/>
     <hyperlink ref="E71" r:id="rId93" xr:uid="{32B8429E-366E-4F53-BE49-98584384E400}"/>
     <hyperlink ref="E72" r:id="rId94" xr:uid="{2F56E697-81C9-4C17-B038-0DEA340DA321}"/>
-    <hyperlink ref="E166" r:id="rId95" xr:uid="{A84E6EB1-7AAD-4E68-B59E-0799174561A9}"/>
+    <hyperlink ref="E170" r:id="rId95" xr:uid="{A84E6EB1-7AAD-4E68-B59E-0799174561A9}"/>
     <hyperlink ref="E73" r:id="rId96" xr:uid="{D05FE410-6952-4A24-9FD1-991C06B5F689}"/>
     <hyperlink ref="E74" r:id="rId97" xr:uid="{0AADED84-1217-4F69-A097-824BE517BAE6}"/>
     <hyperlink ref="E75" r:id="rId98" xr:uid="{F58F404B-B2AB-4AB6-8FD0-CA345BF23295}"/>
-    <hyperlink ref="E176" r:id="rId99" xr:uid="{CF4587E9-BCE0-482F-8792-1ED23D178613}"/>
-    <hyperlink ref="E167" r:id="rId100" xr:uid="{5B60EEEF-58DF-4088-B0B1-1148E588845C}"/>
+    <hyperlink ref="E171" r:id="rId99" xr:uid="{CF4587E9-BCE0-482F-8792-1ED23D178613}"/>
+    <hyperlink ref="E172" r:id="rId100" xr:uid="{5B60EEEF-58DF-4088-B0B1-1148E588845C}"/>
     <hyperlink ref="E76" r:id="rId101" xr:uid="{102AE364-7436-4AD6-B98A-A4E46AE3E2A4}"/>
     <hyperlink ref="E77" r:id="rId102" xr:uid="{A6CA9893-71FC-4567-8D8E-AE7CD0C96307}"/>
     <hyperlink ref="E78" r:id="rId103" xr:uid="{9A05241E-2BBA-4DE7-82F9-27CDC6831D8C}"/>
@@ -52913,13 +52915,13 @@
     <hyperlink ref="E94" r:id="rId119" xr:uid="{CD199838-B14E-4F93-958E-8C87A7F9DA2A}"/>
     <hyperlink ref="E95" r:id="rId120" xr:uid="{E10E96E6-026C-4B6E-896E-B986990DC089}"/>
     <hyperlink ref="E96" r:id="rId121" xr:uid="{BA10BB8E-65EB-4721-A010-203BF9A6A5D2}"/>
-    <hyperlink ref="E168" r:id="rId122" xr:uid="{0B018760-758C-4C50-B09B-C9B9B7F15D0A}"/>
+    <hyperlink ref="E173" r:id="rId122" xr:uid="{0B018760-758C-4C50-B09B-C9B9B7F15D0A}"/>
     <hyperlink ref="E97" r:id="rId123" xr:uid="{55021628-92BB-4771-A925-8E3FBDCBDFB9}"/>
     <hyperlink ref="E98" r:id="rId124" xr:uid="{943387D8-CE78-4A7C-ACFE-ED6DDF1F431A}"/>
     <hyperlink ref="E99" r:id="rId125" xr:uid="{D3928A73-BD52-4C02-AB2F-9853C643E970}"/>
     <hyperlink ref="E100" r:id="rId126" xr:uid="{2E4F5825-A735-431E-9D9E-99DE2E0A3049}"/>
     <hyperlink ref="E101" r:id="rId127" xr:uid="{2D3F3F5B-A835-4B39-984A-EEC22CBF9CF0}"/>
-    <hyperlink ref="E169" r:id="rId128" xr:uid="{B48747D5-B4CC-4269-A066-789011AE64C9}"/>
+    <hyperlink ref="E174" r:id="rId128" xr:uid="{B48747D5-B4CC-4269-A066-789011AE64C9}"/>
     <hyperlink ref="E102" r:id="rId129" xr:uid="{83785163-C660-4443-B521-E03B79573E1E}"/>
     <hyperlink ref="E103" r:id="rId130" xr:uid="{445DC977-38FB-46BF-8D9F-C1644485E94F}"/>
     <hyperlink ref="E104" r:id="rId131" xr:uid="{0F9D2134-7C2F-4435-8510-12D872DE28B9}"/>
@@ -52929,7 +52931,7 @@
     <hyperlink ref="E108" r:id="rId135" xr:uid="{1557C499-DBD1-474F-9632-669E4C5582DD}"/>
     <hyperlink ref="E109" r:id="rId136" xr:uid="{93BD59E0-B0AD-46B1-B78F-381A1AE3DE47}"/>
     <hyperlink ref="E110" r:id="rId137" xr:uid="{60F4C439-9CF6-425F-9789-298A53C71F39}"/>
-    <hyperlink ref="E170" r:id="rId138" xr:uid="{583292B5-CA87-4479-90A8-9AE802612169}"/>
+    <hyperlink ref="E175" r:id="rId138" xr:uid="{583292B5-CA87-4479-90A8-9AE802612169}"/>
     <hyperlink ref="E111" r:id="rId139" xr:uid="{23F3BDB1-5A77-4D93-BE13-5257FF0EC945}"/>
     <hyperlink ref="E113" r:id="rId140" xr:uid="{F7DD7395-D963-403B-881A-9E706FFE7C0F}"/>
     <hyperlink ref="E114" r:id="rId141" xr:uid="{CE8FA04A-13FF-41C7-AFEE-27DA0C243136}"/>
@@ -52945,7 +52947,7 @@
     <hyperlink ref="E124" r:id="rId151" xr:uid="{09E7D3CD-7231-4D38-8626-4C875800492C}"/>
     <hyperlink ref="E125" r:id="rId152" xr:uid="{DFBE85C1-C6C4-4BC3-A284-2104EAB44808}"/>
     <hyperlink ref="E126" r:id="rId153" xr:uid="{5C405DB7-3067-4583-AE30-63D4D583C6A4}"/>
-    <hyperlink ref="E171" r:id="rId154" xr:uid="{B2019643-3B67-45B8-A195-BBC86BB67B42}"/>
+    <hyperlink ref="E176" r:id="rId154" xr:uid="{B2019643-3B67-45B8-A195-BBC86BB67B42}"/>
     <hyperlink ref="E127" r:id="rId155" xr:uid="{18691C8C-80EA-478B-B583-1077747AF0AE}"/>
     <hyperlink ref="E128" r:id="rId156" xr:uid="{608396E6-75C7-4D4C-93E9-2B800FC00E85}"/>
     <hyperlink ref="E129" r:id="rId157" xr:uid="{56CFE394-215C-4353-B707-DCD7D3A65B99}"/>

</xml_diff>